<commit_message>
Added GK removal for iterations
</commit_message>
<xml_diff>
--- a/Player_Analysis/Team_Results.xlsx
+++ b/Player_Analysis/Team_Results.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y24"/>
+  <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,117 +442,97 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Ramón Del Transito Marmolejo</t>
+          <t>Hossam Ayoub</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Eric Mosquera</t>
+          <t>Peter Krüsch</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Gheorghe Tuhuţ</t>
+          <t>Longino Arreola</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Ronny Strande</t>
+          <t>Homero Elías Calles</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Austin Sanders</t>
+          <t>Philip Lehman</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Efraín Cárdenas</t>
+          <t>Phil Peeples</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Matt Mustard-Brown</t>
+          <t>Pacífico Alpízar</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Jarrett Fortier</t>
+          <t>Cole Frampton</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Eleazar Santana</t>
+          <t>Steven Shotwell</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Leider Moncada</t>
+          <t>Roy Belcher</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Brandon Bombard</t>
+          <t>Austin Liner</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Jefferson Long</t>
+          <t>Israel Vernon</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Cliff Shrout</t>
+          <t>Jack McCray</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Brendan Etherton</t>
+          <t>Tom Hayden</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Javier De la Garza</t>
+          <t>Demetrius Machen</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Daniel Farrington</t>
+          <t>Jared Vernon</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Liam Collie</t>
+          <t>Joey Cartwright</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Stuart Bates</t>
+          <t>Mazen Dergham</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Kalin Fischer</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Shane Savoy</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Michael Rudolf Umbach</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Devin Edenfield</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Destin Baum</t>
+          <t>Rogelio Nakamura</t>
         </is>
       </c>
     </row>
@@ -562,77 +542,65 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>FWD</t>
+          <t>FWW</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10.65</v>
+        <v>14.19</v>
       </c>
       <c r="D2" t="n">
-        <v>10.91</v>
+        <v>6.62</v>
       </c>
       <c r="E2" t="n">
-        <v>10.78</v>
+        <v>8.969999999999999</v>
       </c>
       <c r="F2" t="n">
-        <v>11.6</v>
+        <v>9.279999999999999</v>
       </c>
       <c r="G2" t="n">
-        <v>7.62</v>
+        <v>7.56</v>
       </c>
       <c r="H2" t="n">
-        <v>12.05</v>
+        <v>2.4</v>
       </c>
       <c r="I2" t="n">
-        <v>10.76</v>
+        <v>10.21</v>
       </c>
       <c r="J2" t="n">
-        <v>8.960000000000001</v>
+        <v>6.43</v>
       </c>
       <c r="K2" t="n">
-        <v>7.89</v>
+        <v>8.68</v>
       </c>
       <c r="L2" t="n">
-        <v>2.11</v>
+        <v>12.33</v>
       </c>
       <c r="M2" t="n">
-        <v>10.37</v>
+        <v>8.530000000000001</v>
       </c>
       <c r="N2" t="n">
-        <v>7.85</v>
+        <v>6.93</v>
       </c>
       <c r="O2" t="n">
-        <v>8.67</v>
+        <v>2.84</v>
       </c>
       <c r="P2" t="n">
-        <v>9.26</v>
+        <v>9.859999999999999</v>
       </c>
       <c r="Q2" t="n">
-        <v>11.92</v>
+        <v>4.43</v>
       </c>
       <c r="R2" t="n">
-        <v>6.25</v>
+        <v>6.970000000000001</v>
       </c>
       <c r="S2" t="n">
-        <v>9.050000000000001</v>
+        <v>10.74</v>
       </c>
       <c r="T2" t="n">
-        <v>3.05</v>
+        <v>13.26</v>
       </c>
       <c r="U2" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="V2" t="n">
-        <v>5.050000000000001</v>
-      </c>
-      <c r="W2" t="n">
-        <v>9.52</v>
-      </c>
-      <c r="X2" t="n">
-        <v>9.790000000000001</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>1.9</v>
+        <v>4.649999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -641,77 +609,65 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ILRMO</t>
+          <t>FW</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>10.54</v>
+        <v>12.897</v>
       </c>
       <c r="D3" t="n">
-        <v>11.04</v>
+        <v>5.942</v>
       </c>
       <c r="E3" t="n">
-        <v>10.54</v>
+        <v>8.643000000000001</v>
       </c>
       <c r="F3" t="n">
-        <v>11.35</v>
+        <v>7.472</v>
       </c>
       <c r="G3" t="n">
-        <v>9.879999999999999</v>
+        <v>6.622</v>
       </c>
       <c r="H3" t="n">
-        <v>10.33</v>
+        <v>2.141</v>
       </c>
       <c r="I3" t="n">
-        <v>13.04</v>
+        <v>7.892</v>
       </c>
       <c r="J3" t="n">
-        <v>11.57</v>
+        <v>6.512</v>
       </c>
       <c r="K3" t="n">
-        <v>10.97</v>
+        <v>8.402999999999999</v>
       </c>
       <c r="L3" t="n">
-        <v>2.61</v>
+        <v>12.056</v>
       </c>
       <c r="M3" t="n">
-        <v>11.78</v>
+        <v>8.152999999999999</v>
       </c>
       <c r="N3" t="n">
-        <v>12.17</v>
+        <v>4.771000000000001</v>
       </c>
       <c r="O3" t="n">
-        <v>11.98</v>
+        <v>2.631</v>
       </c>
       <c r="P3" t="n">
-        <v>12.13</v>
+        <v>7.953</v>
       </c>
       <c r="Q3" t="n">
-        <v>12.21</v>
+        <v>3.751</v>
       </c>
       <c r="R3" t="n">
-        <v>8.719999999999999</v>
+        <v>5.882</v>
       </c>
       <c r="S3" t="n">
-        <v>10.64</v>
+        <v>8.933</v>
       </c>
       <c r="T3" t="n">
-        <v>4.21</v>
+        <v>12.477</v>
       </c>
       <c r="U3" t="n">
-        <v>8.57</v>
-      </c>
-      <c r="V3" t="n">
-        <v>7.619999999999999</v>
-      </c>
-      <c r="W3" t="n">
-        <v>12.38</v>
-      </c>
-      <c r="X3" t="n">
-        <v>9.969999999999999</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>2.75</v>
+        <v>4.032</v>
       </c>
     </row>
     <row r="4">
@@ -720,77 +676,65 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>FWW</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9.49</v>
+        <v>11.58</v>
       </c>
       <c r="D4" t="n">
-        <v>10.77</v>
+        <v>6.93</v>
       </c>
       <c r="E4" t="n">
-        <v>10.13</v>
+        <v>10.2</v>
       </c>
       <c r="F4" t="n">
-        <v>11.94</v>
+        <v>8.960000000000001</v>
       </c>
       <c r="G4" t="n">
-        <v>7.789999999999999</v>
+        <v>7.76</v>
       </c>
       <c r="H4" t="n">
-        <v>15.85</v>
+        <v>2.11</v>
       </c>
       <c r="I4" t="n">
-        <v>9.5</v>
+        <v>9.68</v>
       </c>
       <c r="J4" t="n">
-        <v>9.279999999999999</v>
+        <v>7.85</v>
       </c>
       <c r="K4" t="n">
-        <v>8.200000000000001</v>
+        <v>9.609999999999999</v>
       </c>
       <c r="L4" t="n">
-        <v>2.4</v>
+        <v>11.92</v>
       </c>
       <c r="M4" t="n">
-        <v>11.38</v>
+        <v>9.26</v>
       </c>
       <c r="N4" t="n">
-        <v>6.43</v>
+        <v>5.69</v>
       </c>
       <c r="O4" t="n">
-        <v>8.24</v>
+        <v>3.05</v>
       </c>
       <c r="P4" t="n">
-        <v>8.530000000000001</v>
+        <v>8.359999999999999</v>
       </c>
       <c r="Q4" t="n">
-        <v>12.33</v>
+        <v>4.119999999999999</v>
       </c>
       <c r="R4" t="n">
-        <v>7.460000000000001</v>
+        <v>6.47</v>
       </c>
       <c r="S4" t="n">
-        <v>11.03</v>
+        <v>10.24</v>
       </c>
       <c r="T4" t="n">
-        <v>2.84</v>
+        <v>10.86</v>
       </c>
       <c r="U4" t="n">
-        <v>5.89</v>
-      </c>
-      <c r="V4" t="n">
-        <v>5.74</v>
-      </c>
-      <c r="W4" t="n">
-        <v>9.809999999999999</v>
-      </c>
-      <c r="X4" t="n">
-        <v>12.18</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>2.02</v>
+        <v>3.87</v>
       </c>
     </row>
     <row r="5">
@@ -799,77 +743,65 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>FW</t>
+          <t>ILRMO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>9.423999999999999</v>
+        <v>10.72</v>
       </c>
       <c r="D5" t="n">
-        <v>9.784000000000001</v>
+        <v>9.57</v>
       </c>
       <c r="E5" t="n">
-        <v>9.603999999999999</v>
+        <v>12.98</v>
       </c>
       <c r="F5" t="n">
-        <v>11.005</v>
+        <v>11.82</v>
       </c>
       <c r="G5" t="n">
-        <v>7.163</v>
+        <v>10.97</v>
       </c>
       <c r="H5" t="n">
-        <v>14.048</v>
+        <v>2.86</v>
       </c>
       <c r="I5" t="n">
-        <v>9.684000000000001</v>
+        <v>11.72</v>
       </c>
       <c r="J5" t="n">
-        <v>7.472</v>
+        <v>12.17</v>
       </c>
       <c r="K5" t="n">
-        <v>6.802</v>
+        <v>12.83</v>
       </c>
       <c r="L5" t="n">
-        <v>2.141</v>
+        <v>12.46</v>
       </c>
       <c r="M5" t="n">
-        <v>9.113</v>
+        <v>12.13</v>
       </c>
       <c r="N5" t="n">
-        <v>6.512</v>
+        <v>8.41</v>
       </c>
       <c r="O5" t="n">
-        <v>7.913</v>
+        <v>4.21</v>
       </c>
       <c r="P5" t="n">
-        <v>8.152999999999999</v>
+        <v>10.33</v>
       </c>
       <c r="Q5" t="n">
-        <v>12.056</v>
+        <v>8.359999999999999</v>
       </c>
       <c r="R5" t="n">
-        <v>5.812</v>
+        <v>9.42</v>
       </c>
       <c r="S5" t="n">
-        <v>9.173999999999999</v>
+        <v>12.28</v>
       </c>
       <c r="T5" t="n">
-        <v>2.631</v>
+        <v>10.82</v>
       </c>
       <c r="U5" t="n">
-        <v>5.212</v>
-      </c>
-      <c r="V5" t="n">
-        <v>4.962</v>
-      </c>
-      <c r="W5" t="n">
-        <v>8.513</v>
-      </c>
-      <c r="X5" t="n">
-        <v>11.807</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>1.35</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="6">
@@ -878,77 +810,65 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ILRM</t>
+          <t>IMW</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>9.19</v>
+        <v>10.39</v>
       </c>
       <c r="D6" t="n">
-        <v>10.37</v>
+        <v>11.52</v>
       </c>
       <c r="E6" t="n">
-        <v>9.19</v>
+        <v>13.26</v>
       </c>
       <c r="F6" t="n">
-        <v>10.59</v>
+        <v>14.49</v>
       </c>
       <c r="G6" t="n">
-        <v>11.15</v>
+        <v>12.77</v>
       </c>
       <c r="H6" t="n">
-        <v>9.48</v>
+        <v>3.74</v>
       </c>
       <c r="I6" t="n">
-        <v>12.78</v>
+        <v>14.72</v>
       </c>
       <c r="J6" t="n">
-        <v>11.75</v>
+        <v>13.06</v>
       </c>
       <c r="K6" t="n">
-        <v>11.75</v>
+        <v>13.05</v>
       </c>
       <c r="L6" t="n">
-        <v>2.99</v>
+        <v>11.22</v>
       </c>
       <c r="M6" t="n">
-        <v>11.56</v>
+        <v>12.72</v>
       </c>
       <c r="N6" t="n">
-        <v>13.34</v>
+        <v>12.75</v>
       </c>
       <c r="O6" t="n">
-        <v>12.38</v>
+        <v>5.42</v>
       </c>
       <c r="P6" t="n">
-        <v>12.56</v>
+        <v>13.05</v>
       </c>
       <c r="Q6" t="n">
-        <v>11.04</v>
+        <v>11.13</v>
       </c>
       <c r="R6" t="n">
-        <v>10.34</v>
+        <v>11.9</v>
       </c>
       <c r="S6" t="n">
-        <v>11.19</v>
+        <v>14.7</v>
       </c>
       <c r="T6" t="n">
-        <v>5.350000000000001</v>
+        <v>10.16</v>
       </c>
       <c r="U6" t="n">
-        <v>10.16</v>
-      </c>
-      <c r="V6" t="n">
-        <v>9.16</v>
-      </c>
-      <c r="W6" t="n">
-        <v>13.15</v>
-      </c>
-      <c r="X6" t="n">
-        <v>9.49</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>2.59</v>
+        <v>3.73</v>
       </c>
     </row>
     <row r="7">
@@ -961,73 +881,61 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>9.18</v>
+        <v>9.719999999999999</v>
       </c>
       <c r="D7" t="n">
-        <v>9.579999999999998</v>
+        <v>8.5</v>
       </c>
       <c r="E7" t="n">
-        <v>9.18</v>
+        <v>11.65</v>
       </c>
       <c r="F7" t="n">
-        <v>9.889999999999999</v>
+        <v>10.67</v>
       </c>
       <c r="G7" t="n">
-        <v>8.809999999999999</v>
+        <v>10</v>
       </c>
       <c r="H7" t="n">
-        <v>9.279999999999999</v>
+        <v>2.53</v>
       </c>
       <c r="I7" t="n">
-        <v>11.76</v>
+        <v>10.39</v>
       </c>
       <c r="J7" t="n">
-        <v>10.47</v>
+        <v>11.15</v>
       </c>
       <c r="K7" t="n">
+        <v>11.73</v>
+      </c>
+      <c r="L7" t="n">
+        <v>11.23</v>
+      </c>
+      <c r="M7" t="n">
+        <v>10.98</v>
+      </c>
+      <c r="N7" t="n">
+        <v>7.52</v>
+      </c>
+      <c r="O7" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="P7" t="n">
+        <v>9.359999999999999</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>7.879999999999999</v>
+      </c>
+      <c r="R7" t="n">
+        <v>8.58</v>
+      </c>
+      <c r="S7" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="T7" t="n">
         <v>10</v>
       </c>
-      <c r="L7" t="n">
-        <v>2.33</v>
-      </c>
-      <c r="M7" t="n">
-        <v>10.5</v>
-      </c>
-      <c r="N7" t="n">
-        <v>11.15</v>
-      </c>
-      <c r="O7" t="n">
-        <v>11.06</v>
-      </c>
-      <c r="P7" t="n">
-        <v>10.98</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>11.03</v>
-      </c>
-      <c r="R7" t="n">
-        <v>7.83</v>
-      </c>
-      <c r="S7" t="n">
-        <v>9.67</v>
-      </c>
-      <c r="T7" t="n">
-        <v>3.6</v>
-      </c>
       <c r="U7" t="n">
-        <v>7.91</v>
-      </c>
-      <c r="V7" t="n">
-        <v>6.960000000000001</v>
-      </c>
-      <c r="W7" t="n">
-        <v>11.18</v>
-      </c>
-      <c r="X7" t="n">
-        <v>9.33</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>2.57</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="8">
@@ -1036,77 +944,65 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>IMW</t>
+          <t>ILRM</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>8.799999999999999</v>
+        <v>9.67</v>
       </c>
       <c r="D8" t="n">
-        <v>11.12</v>
+        <v>10.93</v>
       </c>
       <c r="E8" t="n">
-        <v>9.390000000000001</v>
+        <v>13.15</v>
       </c>
       <c r="F8" t="n">
-        <v>11.12</v>
+        <v>12.34</v>
       </c>
       <c r="G8" t="n">
-        <v>11.52</v>
+        <v>11.75</v>
       </c>
       <c r="H8" t="n">
-        <v>10.65</v>
+        <v>3.58</v>
       </c>
       <c r="I8" t="n">
-        <v>12.1</v>
+        <v>11.93</v>
       </c>
       <c r="J8" t="n">
-        <v>13.92</v>
+        <v>13.34</v>
       </c>
       <c r="K8" t="n">
-        <v>13.36</v>
+        <v>12.97</v>
       </c>
       <c r="L8" t="n">
-        <v>3.17</v>
+        <v>11.63</v>
       </c>
       <c r="M8" t="n">
-        <v>14.15</v>
+        <v>12.56</v>
       </c>
       <c r="N8" t="n">
-        <v>13.06</v>
+        <v>10.12</v>
       </c>
       <c r="O8" t="n">
-        <v>12.51</v>
+        <v>5.350000000000001</v>
       </c>
       <c r="P8" t="n">
-        <v>12.72</v>
+        <v>10.97</v>
       </c>
       <c r="Q8" t="n">
-        <v>10.65</v>
+        <v>10.35</v>
       </c>
       <c r="R8" t="n">
-        <v>12.16</v>
+        <v>10.75</v>
       </c>
       <c r="S8" t="n">
-        <v>13.05</v>
+        <v>12.74</v>
       </c>
       <c r="T8" t="n">
-        <v>5.42</v>
+        <v>10.08</v>
       </c>
       <c r="U8" t="n">
-        <v>10.77</v>
-      </c>
-      <c r="V8" t="n">
-        <v>9.870000000000001</v>
-      </c>
-      <c r="W8" t="n">
-        <v>14.47</v>
-      </c>
-      <c r="X8" t="n">
-        <v>9.029999999999999</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>3.52</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="9">
@@ -1115,77 +1011,65 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ICM</t>
+          <t>W</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8.08</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="D9" t="n">
-        <v>9.06</v>
+        <v>9.709999999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>8.08</v>
+        <v>10.25</v>
       </c>
       <c r="F9" t="n">
-        <v>9.280000000000001</v>
+        <v>12.46</v>
       </c>
       <c r="G9" t="n">
-        <v>9.93</v>
+        <v>10.37</v>
       </c>
       <c r="H9" t="n">
-        <v>8.530000000000001</v>
+        <v>3.33</v>
       </c>
       <c r="I9" t="n">
-        <v>11.6</v>
+        <v>13.24</v>
       </c>
       <c r="J9" t="n">
-        <v>10.7</v>
+        <v>9.649999999999999</v>
       </c>
       <c r="K9" t="n">
-        <v>10.73</v>
+        <v>9.780000000000001</v>
       </c>
       <c r="L9" t="n">
-        <v>2.66</v>
+        <v>8.700000000000001</v>
       </c>
       <c r="M9" t="n">
-        <v>10.38</v>
+        <v>9.880000000000001</v>
       </c>
       <c r="N9" t="n">
-        <v>12.22</v>
+        <v>11.92</v>
       </c>
       <c r="O9" t="n">
-        <v>11.46</v>
+        <v>4.8</v>
       </c>
       <c r="P9" t="n">
-        <v>11.41</v>
+        <v>11.64</v>
       </c>
       <c r="Q9" t="n">
-        <v>10.06</v>
+        <v>8.949999999999999</v>
       </c>
       <c r="R9" t="n">
-        <v>9.25</v>
+        <v>10.1</v>
       </c>
       <c r="S9" t="n">
-        <v>10.17</v>
+        <v>12.93</v>
       </c>
       <c r="T9" t="n">
-        <v>4.59</v>
+        <v>8.27</v>
       </c>
       <c r="U9" t="n">
-        <v>9.300000000000001</v>
-      </c>
-      <c r="V9" t="n">
-        <v>8.300000000000001</v>
-      </c>
-      <c r="W9" t="n">
-        <v>11.9</v>
-      </c>
-      <c r="X9" t="n">
-        <v>8.9</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>2.46</v>
+        <v>3.46</v>
       </c>
     </row>
     <row r="10">
@@ -1194,77 +1078,65 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ILRMD</t>
+          <t>ICM</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>7.31</v>
+        <v>8.82</v>
       </c>
       <c r="D10" t="n">
-        <v>9.01</v>
+        <v>9.709999999999999</v>
       </c>
       <c r="E10" t="n">
-        <v>7.31</v>
+        <v>11.87</v>
       </c>
       <c r="F10" t="n">
-        <v>9.140000000000001</v>
+        <v>11.19</v>
       </c>
       <c r="G10" t="n">
-        <v>11.42</v>
+        <v>10.73</v>
       </c>
       <c r="H10" t="n">
-        <v>8.039999999999999</v>
+        <v>3.15</v>
       </c>
       <c r="I10" t="n">
-        <v>11.54</v>
+        <v>10.65</v>
       </c>
       <c r="J10" t="n">
-        <v>10.96</v>
+        <v>12.22</v>
       </c>
       <c r="K10" t="n">
-        <v>11.49</v>
+        <v>11.92</v>
       </c>
       <c r="L10" t="n">
-        <v>3.1</v>
+        <v>10.55</v>
       </c>
       <c r="M10" t="n">
-        <v>10.46</v>
+        <v>11.41</v>
       </c>
       <c r="N10" t="n">
-        <v>13.29</v>
+        <v>9.029999999999999</v>
       </c>
       <c r="O10" t="n">
-        <v>11.72</v>
+        <v>4.59</v>
       </c>
       <c r="P10" t="n">
-        <v>11.94</v>
+        <v>9.950000000000001</v>
       </c>
       <c r="Q10" t="n">
-        <v>9.15</v>
+        <v>9.620000000000003</v>
       </c>
       <c r="R10" t="n">
-        <v>10.97</v>
+        <v>9.76</v>
       </c>
       <c r="S10" t="n">
-        <v>10.8</v>
+        <v>11.36</v>
       </c>
       <c r="T10" t="n">
-        <v>5.970000000000001</v>
+        <v>9.359999999999999</v>
       </c>
       <c r="U10" t="n">
-        <v>10.75</v>
-      </c>
-      <c r="V10" t="n">
-        <v>9.799999999999997</v>
-      </c>
-      <c r="W10" t="n">
-        <v>12.79</v>
-      </c>
-      <c r="X10" t="n">
-        <v>8.32</v>
-      </c>
-      <c r="Y10" t="n">
-        <v>2.22</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="11">
@@ -1273,77 +1145,65 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>WM</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>6.76</v>
+        <v>8.530000000000001</v>
       </c>
       <c r="D11" t="n">
-        <v>9.58</v>
+        <v>9.440000000000001</v>
       </c>
       <c r="E11" t="n">
-        <v>7.620000000000001</v>
+        <v>10.08</v>
       </c>
       <c r="F11" t="n">
-        <v>9.58</v>
+        <v>11.99</v>
       </c>
       <c r="G11" t="n">
-        <v>9.709999999999999</v>
+        <v>10.2</v>
       </c>
       <c r="H11" t="n">
-        <v>10.01</v>
+        <v>3.22</v>
       </c>
       <c r="I11" t="n">
-        <v>8.84</v>
+        <v>12.49</v>
       </c>
       <c r="J11" t="n">
-        <v>11.91</v>
+        <v>9.81</v>
       </c>
       <c r="K11" t="n">
-        <v>11.23</v>
+        <v>9.780000000000001</v>
       </c>
       <c r="L11" t="n">
-        <v>2.78</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="M11" t="n">
-        <v>12.69</v>
+        <v>9.77</v>
       </c>
       <c r="N11" t="n">
-        <v>9.649999999999999</v>
+        <v>11.35</v>
       </c>
       <c r="O11" t="n">
-        <v>9.409999999999998</v>
+        <v>4.61</v>
       </c>
       <c r="P11" t="n">
+        <v>11.13</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>9.07</v>
+      </c>
+      <c r="R11" t="n">
         <v>9.880000000000001</v>
       </c>
-      <c r="Q11" t="n">
-        <v>8.15</v>
-      </c>
-      <c r="R11" t="n">
-        <v>11.06</v>
-      </c>
       <c r="S11" t="n">
-        <v>11.64</v>
+        <v>12.29</v>
       </c>
       <c r="T11" t="n">
-        <v>4.8</v>
+        <v>8.030000000000001</v>
       </c>
       <c r="U11" t="n">
-        <v>8.870000000000001</v>
-      </c>
-      <c r="V11" t="n">
-        <v>8.42</v>
-      </c>
-      <c r="W11" t="n">
-        <v>12.15</v>
-      </c>
-      <c r="X11" t="n">
-        <v>7.040000000000001</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>2.99</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="12">
@@ -1352,77 +1212,65 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ICMD</t>
+          <t>ILRMD</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>6.56</v>
+        <v>8.01</v>
       </c>
       <c r="D12" t="n">
-        <v>8</v>
+        <v>11.29</v>
       </c>
       <c r="E12" t="n">
-        <v>6.56</v>
+        <v>12.26</v>
       </c>
       <c r="F12" t="n">
-        <v>8.129999999999999</v>
+        <v>11.81</v>
       </c>
       <c r="G12" t="n">
-        <v>10.23</v>
+        <v>11.49</v>
       </c>
       <c r="H12" t="n">
-        <v>7.299999999999999</v>
+        <v>3.95</v>
       </c>
       <c r="I12" t="n">
-        <v>10.6</v>
+        <v>11.18</v>
       </c>
       <c r="J12" t="n">
-        <v>10.09</v>
+        <v>13.29</v>
       </c>
       <c r="K12" t="n">
-        <v>10.56</v>
+        <v>12.04</v>
       </c>
       <c r="L12" t="n">
-        <v>2.77</v>
+        <v>10</v>
       </c>
       <c r="M12" t="n">
-        <v>9.520000000000001</v>
+        <v>11.94</v>
       </c>
       <c r="N12" t="n">
-        <v>12.23</v>
+        <v>10.84</v>
       </c>
       <c r="O12" t="n">
-        <v>10.92</v>
+        <v>5.970000000000001</v>
       </c>
       <c r="P12" t="n">
-        <v>10.94</v>
+        <v>10.67</v>
       </c>
       <c r="Q12" t="n">
-        <v>8.469999999999999</v>
+        <v>11.25</v>
       </c>
       <c r="R12" t="n">
-        <v>9.850000000000001</v>
+        <v>11.07</v>
       </c>
       <c r="S12" t="n">
-        <v>9.869999999999999</v>
+        <v>12.16</v>
       </c>
       <c r="T12" t="n">
-        <v>5.18</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="U12" t="n">
-        <v>9.83</v>
-      </c>
-      <c r="V12" t="n">
-        <v>8.879999999999999</v>
-      </c>
-      <c r="W12" t="n">
-        <v>11.66</v>
-      </c>
-      <c r="X12" t="n">
-        <v>7.85</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>2.15</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="13">
@@ -1431,77 +1279,65 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>WM</t>
+          <t>WD</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>6.380000000000001</v>
+        <v>7.67</v>
       </c>
       <c r="D13" t="n">
-        <v>8.940000000000001</v>
+        <v>10.33</v>
       </c>
       <c r="E13" t="n">
-        <v>7.12</v>
+        <v>9.73</v>
       </c>
       <c r="F13" t="n">
-        <v>8.940000000000001</v>
+        <v>11.54</v>
       </c>
       <c r="G13" t="n">
-        <v>9.440000000000001</v>
+        <v>9.899999999999999</v>
       </c>
       <c r="H13" t="n">
-        <v>9.26</v>
+        <v>3.83</v>
       </c>
       <c r="I13" t="n">
-        <v>8.800000000000001</v>
+        <v>12.19</v>
       </c>
       <c r="J13" t="n">
-        <v>11.45</v>
+        <v>9.68</v>
       </c>
       <c r="K13" t="n">
-        <v>10.94</v>
+        <v>8.91</v>
       </c>
       <c r="L13" t="n">
-        <v>2.68</v>
+        <v>7.71</v>
       </c>
       <c r="M13" t="n">
-        <v>11.95</v>
+        <v>9.469999999999999</v>
       </c>
       <c r="N13" t="n">
-        <v>9.81</v>
+        <v>12.14</v>
       </c>
       <c r="O13" t="n">
-        <v>9.470000000000001</v>
+        <v>5.809999999999999</v>
       </c>
       <c r="P13" t="n">
-        <v>9.77</v>
+        <v>10.98</v>
       </c>
       <c r="Q13" t="n">
-        <v>7.909999999999999</v>
+        <v>9.290000000000001</v>
       </c>
       <c r="R13" t="n">
-        <v>10.61</v>
+        <v>10.2</v>
       </c>
       <c r="S13" t="n">
-        <v>11.13</v>
+        <v>12.36</v>
       </c>
       <c r="T13" t="n">
-        <v>4.61</v>
+        <v>7.02</v>
       </c>
       <c r="U13" t="n">
-        <v>8.83</v>
-      </c>
-      <c r="V13" t="n">
-        <v>8.279999999999999</v>
-      </c>
-      <c r="W13" t="n">
-        <v>11.79</v>
-      </c>
-      <c r="X13" t="n">
-        <v>6.98</v>
-      </c>
-      <c r="Y13" t="n">
-        <v>2.89</v>
+        <v>3.06</v>
       </c>
     </row>
     <row r="14">
@@ -1510,77 +1346,65 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>WD</t>
+          <t>ICMD</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5.819999999999999</v>
+        <v>7.4</v>
       </c>
       <c r="D14" t="n">
-        <v>8.92</v>
+        <v>10.1</v>
       </c>
       <c r="E14" t="n">
-        <v>6.51</v>
+        <v>11.19</v>
       </c>
       <c r="F14" t="n">
-        <v>8.92</v>
+        <v>10.81</v>
       </c>
       <c r="G14" t="n">
-        <v>10.33</v>
+        <v>10.56</v>
       </c>
       <c r="H14" t="n">
-        <v>8.92</v>
+        <v>3.489999999999999</v>
       </c>
       <c r="I14" t="n">
-        <v>8.18</v>
+        <v>10.11</v>
       </c>
       <c r="J14" t="n">
-        <v>10.68</v>
+        <v>12.23</v>
       </c>
       <c r="K14" t="n">
-        <v>10.59</v>
+        <v>11.17</v>
       </c>
       <c r="L14" t="n">
-        <v>2.97</v>
+        <v>9.19</v>
       </c>
       <c r="M14" t="n">
-        <v>11.33</v>
+        <v>10.94</v>
       </c>
       <c r="N14" t="n">
-        <v>9.68</v>
+        <v>9.720000000000001</v>
       </c>
       <c r="O14" t="n">
-        <v>8.649999999999999</v>
+        <v>5.18</v>
       </c>
       <c r="P14" t="n">
-        <v>9.469999999999999</v>
+        <v>9.739999999999998</v>
       </c>
       <c r="Q14" t="n">
-        <v>6.85</v>
+        <v>10.4</v>
       </c>
       <c r="R14" t="n">
-        <v>11.45</v>
+        <v>10.08</v>
       </c>
       <c r="S14" t="n">
-        <v>10.98</v>
+        <v>10.96</v>
       </c>
       <c r="T14" t="n">
-        <v>5.809999999999999</v>
+        <v>8.1</v>
       </c>
       <c r="U14" t="n">
-        <v>9.25</v>
-      </c>
-      <c r="V14" t="n">
-        <v>8.949999999999999</v>
-      </c>
-      <c r="W14" t="n">
-        <v>11.71</v>
-      </c>
-      <c r="X14" t="n">
-        <v>6.07</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>2.24</v>
+        <v>2.43</v>
       </c>
     </row>
     <row r="15">
@@ -1589,77 +1413,65 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>WBM</t>
+          <t>WBO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4.28</v>
+        <v>6.43</v>
       </c>
       <c r="D15" t="n">
-        <v>7.960000000000001</v>
+        <v>10.5</v>
       </c>
       <c r="E15" t="n">
-        <v>4.67</v>
+        <v>8.720000000000001</v>
       </c>
       <c r="F15" t="n">
-        <v>7.960000000000001</v>
+        <v>10.79</v>
       </c>
       <c r="G15" t="n">
-        <v>12.12</v>
+        <v>9.41</v>
       </c>
       <c r="H15" t="n">
-        <v>7.289999999999999</v>
+        <v>4.16</v>
       </c>
       <c r="I15" t="n">
-        <v>7.78</v>
+        <v>11.28</v>
       </c>
       <c r="J15" t="n">
-        <v>9.34</v>
+        <v>9.32</v>
       </c>
       <c r="K15" t="n">
-        <v>10.4</v>
+        <v>7.83</v>
       </c>
       <c r="L15" t="n">
-        <v>3.49</v>
+        <v>6.34</v>
       </c>
       <c r="M15" t="n">
-        <v>9.529999999999999</v>
+        <v>8.720000000000001</v>
       </c>
       <c r="N15" t="n">
-        <v>10.88</v>
+        <v>12.57</v>
       </c>
       <c r="O15" t="n">
-        <v>8.370000000000001</v>
+        <v>6.34</v>
       </c>
       <c r="P15" t="n">
-        <v>9.619999999999999</v>
+        <v>10.59</v>
       </c>
       <c r="Q15" t="n">
-        <v>5.07</v>
+        <v>9.809999999999999</v>
       </c>
       <c r="R15" t="n">
-        <v>12.9</v>
+        <v>10.3</v>
       </c>
       <c r="S15" t="n">
-        <v>10.59</v>
+        <v>11.68</v>
       </c>
       <c r="T15" t="n">
-        <v>7.84</v>
+        <v>5.94</v>
       </c>
       <c r="U15" t="n">
-        <v>10.87</v>
-      </c>
-      <c r="V15" t="n">
-        <v>10.67</v>
-      </c>
-      <c r="W15" t="n">
-        <v>11.85</v>
-      </c>
-      <c r="X15" t="n">
-        <v>5.07</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>1.18</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="16">
@@ -1672,73 +1484,61 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4.23</v>
+        <v>6.15</v>
       </c>
       <c r="D16" t="n">
-        <v>8.01</v>
+        <v>11.47</v>
       </c>
       <c r="E16" t="n">
-        <v>4.82</v>
+        <v>9.17</v>
       </c>
       <c r="F16" t="n">
-        <v>8.01</v>
+        <v>10.94</v>
       </c>
       <c r="G16" t="n">
-        <v>11.47</v>
+        <v>9.76</v>
       </c>
       <c r="H16" t="n">
-        <v>7.890000000000001</v>
+        <v>4.640000000000001</v>
       </c>
       <c r="I16" t="n">
-        <v>7.279999999999999</v>
+        <v>11.38</v>
       </c>
       <c r="J16" t="n">
-        <v>9.640000000000001</v>
+        <v>10.03</v>
       </c>
       <c r="K16" t="n">
-        <v>10.35</v>
+        <v>8.02</v>
       </c>
       <c r="L16" t="n">
-        <v>3.34</v>
+        <v>6.42</v>
       </c>
       <c r="M16" t="n">
-        <v>10.08</v>
+        <v>9.17</v>
       </c>
       <c r="N16" t="n">
-        <v>10.03</v>
+        <v>13.24</v>
       </c>
       <c r="O16" t="n">
-        <v>8.02</v>
+        <v>7.24</v>
       </c>
       <c r="P16" t="n">
-        <v>9.17</v>
+        <v>10.79</v>
       </c>
       <c r="Q16" t="n">
-        <v>5.12</v>
+        <v>10.47</v>
       </c>
       <c r="R16" t="n">
-        <v>12.65</v>
+        <v>10.91</v>
       </c>
       <c r="S16" t="n">
-        <v>10.79</v>
+        <v>12.09</v>
       </c>
       <c r="T16" t="n">
-        <v>7.24</v>
+        <v>5.71</v>
       </c>
       <c r="U16" t="n">
-        <v>10.32</v>
-      </c>
-      <c r="V16" t="n">
-        <v>10.17</v>
-      </c>
-      <c r="W16" t="n">
-        <v>11.65</v>
-      </c>
-      <c r="X16" t="n">
-        <v>5.12</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>1.48</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="17">
@@ -1751,73 +1551,61 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4.19</v>
+        <v>6.12</v>
       </c>
       <c r="D17" t="n">
-        <v>6.19</v>
+        <v>8.32</v>
       </c>
       <c r="E17" t="n">
-        <v>4.59</v>
+        <v>8.58</v>
       </c>
       <c r="F17" t="n">
-        <v>6.19</v>
+        <v>9.780000000000001</v>
       </c>
       <c r="G17" t="n">
-        <v>8.32</v>
+        <v>8.98</v>
       </c>
       <c r="H17" t="n">
-        <v>6.390000000000001</v>
+        <v>2.93</v>
       </c>
       <c r="I17" t="n">
-        <v>7.58</v>
+        <v>9.450000000000001</v>
       </c>
       <c r="J17" t="n">
+        <v>9.510000000000002</v>
+      </c>
+      <c r="K17" t="n">
+        <v>8.710000000000001</v>
+      </c>
+      <c r="L17" t="n">
+        <v>6.65</v>
+      </c>
+      <c r="M17" t="n">
+        <v>8.58</v>
+      </c>
+      <c r="N17" t="n">
+        <v>9.52</v>
+      </c>
+      <c r="O17" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="P17" t="n">
+        <v>9.050000000000001</v>
+      </c>
+      <c r="Q17" t="n">
         <v>9.18</v>
       </c>
-      <c r="K17" t="n">
-        <v>9.379999999999999</v>
-      </c>
-      <c r="L17" t="n">
-        <v>2.33</v>
-      </c>
-      <c r="M17" t="n">
-        <v>8.850000000000001</v>
-      </c>
-      <c r="N17" t="n">
-        <v>9.510000000000002</v>
-      </c>
-      <c r="O17" t="n">
-        <v>8.710000000000001</v>
-      </c>
-      <c r="P17" t="n">
-        <v>8.58</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>6.05</v>
-      </c>
       <c r="R17" t="n">
-        <v>9.120000000000001</v>
+        <v>8.85</v>
       </c>
       <c r="S17" t="n">
-        <v>9.050000000000001</v>
+        <v>9.65</v>
       </c>
       <c r="T17" t="n">
-        <v>4.13</v>
+        <v>6.449999999999999</v>
       </c>
       <c r="U17" t="n">
-        <v>8.449999999999999</v>
-      </c>
-      <c r="V17" t="n">
-        <v>7.720000000000001</v>
-      </c>
-      <c r="W17" t="n">
-        <v>9.98</v>
-      </c>
-      <c r="X17" t="n">
-        <v>6.05</v>
-      </c>
-      <c r="Y17" t="n">
-        <v>2.26</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="18">
@@ -1826,77 +1614,65 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>WBO</t>
+          <t>WBM</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4.16</v>
+        <v>5.65</v>
       </c>
       <c r="D18" t="n">
-        <v>7.719999999999999</v>
+        <v>12.12</v>
       </c>
       <c r="E18" t="n">
-        <v>4.85</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="F18" t="n">
-        <v>7.719999999999999</v>
+        <v>10.79</v>
       </c>
       <c r="G18" t="n">
-        <v>10.5</v>
+        <v>10.01</v>
       </c>
       <c r="H18" t="n">
-        <v>8.01</v>
+        <v>4.94</v>
       </c>
       <c r="I18" t="n">
-        <v>6.94</v>
+        <v>10.98</v>
       </c>
       <c r="J18" t="n">
-        <v>9.699999999999999</v>
+        <v>10.88</v>
       </c>
       <c r="K18" t="n">
-        <v>10.1</v>
+        <v>8.370000000000001</v>
       </c>
       <c r="L18" t="n">
-        <v>3.07</v>
+        <v>6.52</v>
       </c>
       <c r="M18" t="n">
-        <v>10.19</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="N18" t="n">
-        <v>9.32</v>
+        <v>13.29</v>
       </c>
       <c r="O18" t="n">
-        <v>7.83</v>
+        <v>7.84</v>
       </c>
       <c r="P18" t="n">
-        <v>8.720000000000001</v>
+        <v>10.59</v>
       </c>
       <c r="Q18" t="n">
-        <v>5.25</v>
+        <v>11.07</v>
       </c>
       <c r="R18" t="n">
-        <v>11.88</v>
+        <v>11.26</v>
       </c>
       <c r="S18" t="n">
-        <v>10.59</v>
+        <v>12.04</v>
       </c>
       <c r="T18" t="n">
-        <v>6.34</v>
+        <v>5.46</v>
       </c>
       <c r="U18" t="n">
-        <v>9.609999999999999</v>
-      </c>
-      <c r="V18" t="n">
-        <v>9.409999999999998</v>
-      </c>
-      <c r="W18" t="n">
-        <v>11.19</v>
-      </c>
-      <c r="X18" t="n">
-        <v>5.25</v>
-      </c>
-      <c r="Y18" t="n">
-        <v>1.78</v>
+        <v>2.43</v>
       </c>
     </row>
     <row r="19">
@@ -1909,73 +1685,61 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4.06</v>
+        <v>5.51</v>
       </c>
       <c r="D19" t="n">
-        <v>7.819999999999999</v>
+        <v>11.76</v>
       </c>
       <c r="E19" t="n">
-        <v>4.51</v>
+        <v>9.1</v>
       </c>
       <c r="F19" t="n">
-        <v>7.819999999999999</v>
+        <v>10.45</v>
       </c>
       <c r="G19" t="n">
-        <v>11.76</v>
+        <v>9.550000000000001</v>
       </c>
       <c r="H19" t="n">
-        <v>7.29</v>
+        <v>4.84</v>
       </c>
       <c r="I19" t="n">
-        <v>7.220000000000001</v>
+        <v>10.8</v>
       </c>
       <c r="J19" t="n">
-        <v>9.02</v>
+        <v>10.18</v>
       </c>
       <c r="K19" t="n">
-        <v>10</v>
+        <v>7.77</v>
       </c>
       <c r="L19" t="n">
-        <v>3.41</v>
+        <v>6.140000000000001</v>
       </c>
       <c r="M19" t="n">
-        <v>9.369999999999999</v>
+        <v>9.1</v>
       </c>
       <c r="N19" t="n">
-        <v>10.18</v>
+        <v>13.11</v>
       </c>
       <c r="O19" t="n">
-        <v>7.77</v>
+        <v>7.7</v>
       </c>
       <c r="P19" t="n">
-        <v>9.1</v>
+        <v>10.35</v>
       </c>
       <c r="Q19" t="n">
-        <v>4.71</v>
+        <v>10.53</v>
       </c>
       <c r="R19" t="n">
-        <v>12.66</v>
+        <v>10.88</v>
       </c>
       <c r="S19" t="n">
-        <v>10.35</v>
+        <v>11.78</v>
       </c>
       <c r="T19" t="n">
-        <v>7.7</v>
+        <v>5.16</v>
       </c>
       <c r="U19" t="n">
-        <v>10.43</v>
-      </c>
-      <c r="V19" t="n">
-        <v>10.33</v>
-      </c>
-      <c r="W19" t="n">
-        <v>11.43</v>
-      </c>
-      <c r="X19" t="n">
-        <v>4.71</v>
-      </c>
-      <c r="Y19" t="n">
-        <v>1.1</v>
+        <v>2.43</v>
       </c>
     </row>
     <row r="20">
@@ -1988,73 +1752,61 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3.93</v>
+        <v>4.86</v>
       </c>
       <c r="D20" t="n">
-        <v>7.41</v>
+        <v>11.74</v>
       </c>
       <c r="E20" t="n">
-        <v>4.19</v>
+        <v>9.08</v>
       </c>
       <c r="F20" t="n">
-        <v>7.41</v>
+        <v>9.860000000000001</v>
       </c>
       <c r="G20" t="n">
-        <v>11.74</v>
+        <v>9.34</v>
       </c>
       <c r="H20" t="n">
-        <v>6.450000000000001</v>
+        <v>4.850000000000001</v>
       </c>
       <c r="I20" t="n">
-        <v>7.34</v>
+        <v>9.970000000000001</v>
       </c>
       <c r="J20" t="n">
-        <v>8.380000000000001</v>
+        <v>10.45</v>
       </c>
       <c r="K20" t="n">
-        <v>9.600000000000001</v>
+        <v>7.75</v>
       </c>
       <c r="L20" t="n">
-        <v>3.37</v>
+        <v>5.970000000000001</v>
       </c>
       <c r="M20" t="n">
-        <v>8.49</v>
+        <v>9.08</v>
       </c>
       <c r="N20" t="n">
-        <v>10.45</v>
+        <v>12.52</v>
       </c>
       <c r="O20" t="n">
-        <v>7.75</v>
+        <v>7.81</v>
       </c>
       <c r="P20" t="n">
-        <v>9.08</v>
+        <v>9.710000000000001</v>
       </c>
       <c r="Q20" t="n">
-        <v>4.49</v>
+        <v>10.56</v>
       </c>
       <c r="R20" t="n">
-        <v>12.26</v>
+        <v>10.67</v>
       </c>
       <c r="S20" t="n">
-        <v>9.710000000000001</v>
+        <v>11.19</v>
       </c>
       <c r="T20" t="n">
-        <v>7.81</v>
+        <v>4.75</v>
       </c>
       <c r="U20" t="n">
-        <v>10.41</v>
-      </c>
-      <c r="V20" t="n">
-        <v>10.26</v>
-      </c>
-      <c r="W20" t="n">
-        <v>11.08</v>
-      </c>
-      <c r="X20" t="n">
-        <v>4.49</v>
-      </c>
-      <c r="Y20" t="n">
-        <v>0.8200000000000001</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="21">
@@ -2063,77 +1815,65 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CLRD</t>
+          <t>WO</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3.79</v>
+        <v>4.5</v>
       </c>
       <c r="D21" t="n">
-        <v>6.83</v>
+        <v>5.630000000000001</v>
       </c>
       <c r="E21" t="n">
-        <v>3.79</v>
+        <v>6.37</v>
       </c>
       <c r="F21" t="n">
-        <v>6.83</v>
+        <v>6.25</v>
       </c>
       <c r="G21" t="n">
-        <v>11.64</v>
+        <v>5.629999999999999</v>
       </c>
       <c r="H21" t="n">
-        <v>5.31</v>
+        <v>1.87</v>
       </c>
       <c r="I21" t="n">
-        <v>7.58</v>
+        <v>6.47</v>
       </c>
       <c r="J21" t="n">
-        <v>7.58</v>
+        <v>6.08</v>
       </c>
       <c r="K21" t="n">
-        <v>9.1</v>
+        <v>5.9</v>
       </c>
       <c r="L21" t="n">
-        <v>3.29</v>
+        <v>5.37</v>
       </c>
       <c r="M21" t="n">
-        <v>7.33</v>
+        <v>5.95</v>
       </c>
       <c r="N21" t="n">
-        <v>10.87</v>
+        <v>5.51</v>
       </c>
       <c r="O21" t="n">
-        <v>7.83</v>
+        <v>2.989999999999999</v>
       </c>
       <c r="P21" t="n">
-        <v>9.1</v>
+        <v>5.529999999999999</v>
       </c>
       <c r="Q21" t="n">
-        <v>4.29</v>
+        <v>4.62</v>
       </c>
       <c r="R21" t="n">
-        <v>11.64</v>
+        <v>5.26</v>
       </c>
       <c r="S21" t="n">
-        <v>8.85</v>
+        <v>6.72</v>
       </c>
       <c r="T21" t="n">
-        <v>7.85</v>
+        <v>4.28</v>
       </c>
       <c r="U21" t="n">
-        <v>10.37</v>
-      </c>
-      <c r="V21" t="n">
-        <v>10.12</v>
-      </c>
-      <c r="W21" t="n">
-        <v>10.62</v>
-      </c>
-      <c r="X21" t="n">
-        <v>4.29</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>0.5</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="22">
@@ -2142,77 +1882,65 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>CCD</t>
+          <t>CLRD</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3.27</v>
+        <v>4.04</v>
       </c>
       <c r="D22" t="n">
-        <v>5.79</v>
+        <v>11.64</v>
       </c>
       <c r="E22" t="n">
-        <v>3.27</v>
+        <v>9.1</v>
       </c>
       <c r="F22" t="n">
-        <v>5.79</v>
+        <v>9.1</v>
       </c>
       <c r="G22" t="n">
-        <v>9.82</v>
+        <v>9.1</v>
       </c>
       <c r="H22" t="n">
-        <v>4.53</v>
+        <v>4.81</v>
       </c>
       <c r="I22" t="n">
-        <v>6.54</v>
+        <v>8.85</v>
       </c>
       <c r="J22" t="n">
-        <v>6.54</v>
+        <v>10.87</v>
       </c>
       <c r="K22" t="n">
-        <v>7.8</v>
+        <v>7.83</v>
       </c>
       <c r="L22" t="n">
-        <v>2.77</v>
+        <v>5.81</v>
       </c>
       <c r="M22" t="n">
-        <v>6.29</v>
+        <v>9.1</v>
       </c>
       <c r="N22" t="n">
-        <v>9.31</v>
+        <v>11.64</v>
       </c>
       <c r="O22" t="n">
-        <v>6.79</v>
+        <v>7.85</v>
       </c>
       <c r="P22" t="n">
-        <v>7.8</v>
+        <v>8.85</v>
       </c>
       <c r="Q22" t="n">
-        <v>3.77</v>
+        <v>10.62</v>
       </c>
       <c r="R22" t="n">
-        <v>9.82</v>
+        <v>10.37</v>
       </c>
       <c r="S22" t="n">
-        <v>7.55</v>
+        <v>10.37</v>
       </c>
       <c r="T22" t="n">
-        <v>6.55</v>
+        <v>4.29</v>
       </c>
       <c r="U22" t="n">
-        <v>8.81</v>
-      </c>
-      <c r="V22" t="n">
-        <v>8.56</v>
-      </c>
-      <c r="W22" t="n">
-        <v>9.06</v>
-      </c>
-      <c r="X22" t="n">
-        <v>3.77</v>
-      </c>
-      <c r="Y22" t="n">
-        <v>0.5</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="23">
@@ -2221,77 +1949,65 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>GK</t>
+          <t>CCD</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2.68</v>
+        <v>3.52</v>
       </c>
       <c r="D23" t="n">
-        <v>3.88</v>
+        <v>9.82</v>
       </c>
       <c r="E23" t="n">
-        <v>2.68</v>
+        <v>7.8</v>
       </c>
       <c r="F23" t="n">
-        <v>3.88</v>
+        <v>7.8</v>
       </c>
       <c r="G23" t="n">
-        <v>5.68</v>
+        <v>7.8</v>
       </c>
       <c r="H23" t="n">
-        <v>3.28</v>
+        <v>4.03</v>
       </c>
       <c r="I23" t="n">
-        <v>3.88</v>
+        <v>7.55</v>
       </c>
       <c r="J23" t="n">
-        <v>3.88</v>
+        <v>9.31</v>
       </c>
       <c r="K23" t="n">
-        <v>4.48</v>
+        <v>6.79</v>
       </c>
       <c r="L23" t="n">
-        <v>10.08</v>
+        <v>5.03</v>
       </c>
       <c r="M23" t="n">
-        <v>3.88</v>
+        <v>7.8</v>
       </c>
       <c r="N23" t="n">
-        <v>5.08</v>
+        <v>9.82</v>
       </c>
       <c r="O23" t="n">
-        <v>3.88</v>
+        <v>6.55</v>
       </c>
       <c r="P23" t="n">
-        <v>5.96</v>
+        <v>7.55</v>
       </c>
       <c r="Q23" t="n">
-        <v>2.68</v>
+        <v>9.06</v>
       </c>
       <c r="R23" t="n">
-        <v>5.68</v>
+        <v>8.81</v>
       </c>
       <c r="S23" t="n">
-        <v>4.48</v>
+        <v>8.81</v>
       </c>
       <c r="T23" t="n">
-        <v>11.88</v>
+        <v>3.77</v>
       </c>
       <c r="U23" t="n">
-        <v>5.08</v>
-      </c>
-      <c r="V23" t="n">
-        <v>5.08</v>
-      </c>
-      <c r="W23" t="n">
-        <v>6.56</v>
-      </c>
-      <c r="X23" t="n">
-        <v>2.68</v>
-      </c>
-      <c r="Y23" t="n">
-        <v>2.96</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="24">
@@ -2300,120 +2016,66 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>LAST</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>FW</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>FW</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>FW</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>FW</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>CD</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>FW</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>FW</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>IM</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>LW</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
           <t>GK</t>
         </is>
       </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>RW</t>
-        </is>
-      </c>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>CD</t>
-        </is>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>IM</t>
-        </is>
-      </c>
-      <c r="P24" t="inlineStr">
-        <is>
-          <t>IM</t>
-        </is>
-      </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>IM</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>LB</t>
-        </is>
-      </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>LW</t>
-        </is>
-      </c>
-      <c r="T24" t="inlineStr">
-        <is>
-          <t>GK</t>
-        </is>
-      </c>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>CD</t>
-        </is>
-      </c>
-      <c r="V24" t="inlineStr">
-        <is>
-          <t>CD</t>
-        </is>
-      </c>
-      <c r="W24" t="inlineStr">
-        <is>
-          <t>CD</t>
-        </is>
-      </c>
-      <c r="X24" t="inlineStr">
-        <is>
-          <t>IM</t>
-        </is>
-      </c>
-      <c r="Y24" t="inlineStr"/>
+      <c r="C24" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="D24" t="n">
+        <v>5.68</v>
+      </c>
+      <c r="E24" t="n">
+        <v>4.48</v>
+      </c>
+      <c r="F24" t="n">
+        <v>4.48</v>
+      </c>
+      <c r="G24" t="n">
+        <v>4.48</v>
+      </c>
+      <c r="H24" t="n">
+        <v>10.68</v>
+      </c>
+      <c r="I24" t="n">
+        <v>4.48</v>
+      </c>
+      <c r="J24" t="n">
+        <v>5.08</v>
+      </c>
+      <c r="K24" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="L24" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="M24" t="n">
+        <v>5.96</v>
+      </c>
+      <c r="N24" t="n">
+        <v>5.68</v>
+      </c>
+      <c r="O24" t="n">
+        <v>11.88</v>
+      </c>
+      <c r="P24" t="n">
+        <v>4.48</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>5.08</v>
+      </c>
+      <c r="R24" t="n">
+        <v>5.08</v>
+      </c>
+      <c r="S24" t="n">
+        <v>6.56</v>
+      </c>
+      <c r="T24" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="U24" t="n">
+        <v>3.56</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated Entry to auto select two lineups after iterations
</commit_message>
<xml_diff>
--- a/Player_Analysis/Team_Results.xlsx
+++ b/Player_Analysis/Team_Results.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U24"/>
+  <dimension ref="A1:AE24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,95 +442,145 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Leopold Vach</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Daniele Passarin</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Sergiusz Soplica</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Samuele Camaiani</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Giovanni Plazas</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Yuanfu Fu</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>František Panec</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Andrei Dochioiu</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Achikam Givon</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Detlef Wetter</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>Hossam Ayoub</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Peter Krüsch</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Longino Arreola</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Homero Elías Calles</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Philip Lehman</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Phil Peeples</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Pacífico Alpízar</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Cole Frampton</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Steven Shotwell</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Roy Belcher</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Austin Liner</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Israel Vernon</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Jack McCray</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Tom Hayden</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Demetrius Machen</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Jared Vernon</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Joey Cartwright</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Mazen Dergham</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Rogelio Nakamura</t>
         </is>
@@ -542,65 +592,95 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>FWW</t>
+          <t>IMW</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>14.19</v>
+        <v>13.59</v>
       </c>
       <c r="D2" t="n">
-        <v>6.62</v>
+        <v>11.84</v>
       </c>
       <c r="E2" t="n">
-        <v>8.969999999999999</v>
+        <v>11.32</v>
       </c>
       <c r="F2" t="n">
-        <v>9.279999999999999</v>
+        <v>11.94</v>
       </c>
       <c r="G2" t="n">
-        <v>7.56</v>
+        <v>12.41</v>
       </c>
       <c r="H2" t="n">
-        <v>2.4</v>
+        <v>11.68</v>
       </c>
       <c r="I2" t="n">
-        <v>10.21</v>
+        <v>11.63</v>
       </c>
       <c r="J2" t="n">
-        <v>6.43</v>
+        <v>14.16</v>
       </c>
       <c r="K2" t="n">
-        <v>8.68</v>
+        <v>13.31</v>
       </c>
       <c r="L2" t="n">
-        <v>12.33</v>
+        <v>11.84</v>
       </c>
       <c r="M2" t="n">
-        <v>8.530000000000001</v>
+        <v>10.39</v>
       </c>
       <c r="N2" t="n">
-        <v>6.93</v>
+        <v>11.52</v>
       </c>
       <c r="O2" t="n">
-        <v>2.84</v>
+        <v>13.26</v>
       </c>
       <c r="P2" t="n">
-        <v>9.859999999999999</v>
+        <v>14.49</v>
       </c>
       <c r="Q2" t="n">
-        <v>4.43</v>
+        <v>12.77</v>
       </c>
       <c r="R2" t="n">
-        <v>6.970000000000001</v>
+        <v>3.74</v>
       </c>
       <c r="S2" t="n">
-        <v>10.74</v>
+        <v>14.72</v>
       </c>
       <c r="T2" t="n">
-        <v>13.26</v>
+        <v>13.06</v>
       </c>
       <c r="U2" t="n">
-        <v>4.649999999999999</v>
+        <v>13.05</v>
+      </c>
+      <c r="V2" t="n">
+        <v>11.22</v>
+      </c>
+      <c r="W2" t="n">
+        <v>12.72</v>
+      </c>
+      <c r="X2" t="n">
+        <v>12.75</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>5.42</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>13.05</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>11.13</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>11.9</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>10.16</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>3.73</v>
       </c>
     </row>
     <row r="3">
@@ -609,65 +689,95 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>FW</t>
+          <t>FWW</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>12.897</v>
+        <v>12.64</v>
       </c>
       <c r="D3" t="n">
-        <v>5.942</v>
+        <v>11.36</v>
       </c>
       <c r="E3" t="n">
-        <v>8.643000000000001</v>
+        <v>9.220000000000001</v>
       </c>
       <c r="F3" t="n">
-        <v>7.472</v>
+        <v>9.42</v>
       </c>
       <c r="G3" t="n">
-        <v>6.622</v>
+        <v>9.02</v>
       </c>
       <c r="H3" t="n">
-        <v>2.141</v>
+        <v>8.93</v>
       </c>
       <c r="I3" t="n">
-        <v>7.892</v>
+        <v>11.07</v>
       </c>
       <c r="J3" t="n">
-        <v>6.512</v>
+        <v>10.3</v>
       </c>
       <c r="K3" t="n">
-        <v>8.402999999999999</v>
+        <v>11.51</v>
       </c>
       <c r="L3" t="n">
-        <v>12.056</v>
+        <v>11.36</v>
       </c>
       <c r="M3" t="n">
-        <v>8.152999999999999</v>
+        <v>14.19</v>
       </c>
       <c r="N3" t="n">
-        <v>4.771000000000001</v>
+        <v>6.62</v>
       </c>
       <c r="O3" t="n">
-        <v>2.631</v>
+        <v>8.969999999999999</v>
       </c>
       <c r="P3" t="n">
-        <v>7.953</v>
+        <v>9.279999999999999</v>
       </c>
       <c r="Q3" t="n">
-        <v>3.751</v>
+        <v>7.56</v>
       </c>
       <c r="R3" t="n">
-        <v>5.882</v>
+        <v>2.4</v>
       </c>
       <c r="S3" t="n">
-        <v>8.933</v>
+        <v>10.21</v>
       </c>
       <c r="T3" t="n">
-        <v>12.477</v>
+        <v>6.43</v>
       </c>
       <c r="U3" t="n">
-        <v>4.032</v>
+        <v>8.68</v>
+      </c>
+      <c r="V3" t="n">
+        <v>12.33</v>
+      </c>
+      <c r="W3" t="n">
+        <v>8.530000000000001</v>
+      </c>
+      <c r="X3" t="n">
+        <v>6.93</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>9.859999999999999</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>6.970000000000001</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>10.74</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>13.26</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>4.649999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -676,65 +786,95 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>FWD</t>
+          <t>W</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>11.58</v>
+        <v>12.01</v>
       </c>
       <c r="D4" t="n">
-        <v>6.93</v>
+        <v>9.740000000000002</v>
       </c>
       <c r="E4" t="n">
-        <v>10.2</v>
+        <v>9.68</v>
       </c>
       <c r="F4" t="n">
-        <v>8.960000000000001</v>
+        <v>10.72</v>
       </c>
       <c r="G4" t="n">
-        <v>7.76</v>
+        <v>10.29</v>
       </c>
       <c r="H4" t="n">
-        <v>2.11</v>
+        <v>9.76</v>
       </c>
       <c r="I4" t="n">
-        <v>9.68</v>
+        <v>9.27</v>
       </c>
       <c r="J4" t="n">
-        <v>7.85</v>
+        <v>12.56</v>
       </c>
       <c r="K4" t="n">
-        <v>9.609999999999999</v>
+        <v>10.74</v>
       </c>
       <c r="L4" t="n">
+        <v>9.740000000000002</v>
+      </c>
+      <c r="M4" t="n">
+        <v>9.050000000000001</v>
+      </c>
+      <c r="N4" t="n">
+        <v>9.709999999999999</v>
+      </c>
+      <c r="O4" t="n">
+        <v>10.25</v>
+      </c>
+      <c r="P4" t="n">
+        <v>12.46</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>10.37</v>
+      </c>
+      <c r="R4" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="S4" t="n">
+        <v>13.24</v>
+      </c>
+      <c r="T4" t="n">
+        <v>9.649999999999999</v>
+      </c>
+      <c r="U4" t="n">
+        <v>9.780000000000001</v>
+      </c>
+      <c r="V4" t="n">
+        <v>8.700000000000001</v>
+      </c>
+      <c r="W4" t="n">
+        <v>9.880000000000001</v>
+      </c>
+      <c r="X4" t="n">
         <v>11.92</v>
       </c>
-      <c r="M4" t="n">
-        <v>9.26</v>
-      </c>
-      <c r="N4" t="n">
-        <v>5.69</v>
-      </c>
-      <c r="O4" t="n">
-        <v>3.05</v>
-      </c>
-      <c r="P4" t="n">
-        <v>8.359999999999999</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>4.119999999999999</v>
-      </c>
-      <c r="R4" t="n">
-        <v>6.47</v>
-      </c>
-      <c r="S4" t="n">
-        <v>10.24</v>
-      </c>
-      <c r="T4" t="n">
-        <v>10.86</v>
-      </c>
-      <c r="U4" t="n">
-        <v>3.87</v>
+      <c r="Y4" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>11.64</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>8.949999999999999</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>12.93</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>8.27</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>3.46</v>
       </c>
     </row>
     <row r="5">
@@ -743,65 +883,95 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ILRMO</t>
+          <t>ILRM</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>10.72</v>
+        <v>12</v>
       </c>
       <c r="D5" t="n">
-        <v>9.57</v>
+        <v>11.41</v>
       </c>
       <c r="E5" t="n">
-        <v>12.98</v>
+        <v>9.790000000000001</v>
       </c>
       <c r="F5" t="n">
-        <v>11.82</v>
+        <v>9.790000000000001</v>
       </c>
       <c r="G5" t="n">
+        <v>11.56</v>
+      </c>
+      <c r="H5" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>11.23</v>
+      </c>
+      <c r="J5" t="n">
+        <v>12.15</v>
+      </c>
+      <c r="K5" t="n">
+        <v>13</v>
+      </c>
+      <c r="L5" t="n">
+        <v>11.41</v>
+      </c>
+      <c r="M5" t="n">
+        <v>9.67</v>
+      </c>
+      <c r="N5" t="n">
+        <v>10.93</v>
+      </c>
+      <c r="O5" t="n">
+        <v>13.15</v>
+      </c>
+      <c r="P5" t="n">
+        <v>12.34</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>11.75</v>
+      </c>
+      <c r="R5" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="S5" t="n">
+        <v>11.93</v>
+      </c>
+      <c r="T5" t="n">
+        <v>13.34</v>
+      </c>
+      <c r="U5" t="n">
+        <v>12.97</v>
+      </c>
+      <c r="V5" t="n">
+        <v>11.63</v>
+      </c>
+      <c r="W5" t="n">
+        <v>12.56</v>
+      </c>
+      <c r="X5" t="n">
+        <v>10.12</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>5.350000000000001</v>
+      </c>
+      <c r="Z5" t="n">
         <v>10.97</v>
       </c>
-      <c r="H5" t="n">
-        <v>2.86</v>
-      </c>
-      <c r="I5" t="n">
-        <v>11.72</v>
-      </c>
-      <c r="J5" t="n">
-        <v>12.17</v>
-      </c>
-      <c r="K5" t="n">
-        <v>12.83</v>
-      </c>
-      <c r="L5" t="n">
-        <v>12.46</v>
-      </c>
-      <c r="M5" t="n">
-        <v>12.13</v>
-      </c>
-      <c r="N5" t="n">
-        <v>8.41</v>
-      </c>
-      <c r="O5" t="n">
-        <v>4.21</v>
-      </c>
-      <c r="P5" t="n">
-        <v>10.33</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>8.359999999999999</v>
-      </c>
-      <c r="R5" t="n">
-        <v>9.42</v>
-      </c>
-      <c r="S5" t="n">
-        <v>12.28</v>
-      </c>
-      <c r="T5" t="n">
-        <v>10.82</v>
-      </c>
-      <c r="U5" t="n">
-        <v>3.52</v>
+      <c r="AA5" t="n">
+        <v>10.35</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>10.75</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>12.74</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>10.08</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>3.21</v>
       </c>
     </row>
     <row r="6">
@@ -810,65 +980,95 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>IMW</t>
+          <t>ILRMO</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>10.39</v>
+        <v>11.8</v>
       </c>
       <c r="D6" t="n">
-        <v>11.52</v>
+        <v>11.55</v>
       </c>
       <c r="E6" t="n">
-        <v>13.26</v>
+        <v>9.829999999999998</v>
       </c>
       <c r="F6" t="n">
-        <v>14.49</v>
+        <v>9.23</v>
       </c>
       <c r="G6" t="n">
-        <v>12.77</v>
+        <v>11.18</v>
       </c>
       <c r="H6" t="n">
-        <v>3.74</v>
+        <v>9.93</v>
       </c>
       <c r="I6" t="n">
-        <v>14.72</v>
+        <v>11.4</v>
       </c>
       <c r="J6" t="n">
-        <v>13.06</v>
+        <v>11.43</v>
       </c>
       <c r="K6" t="n">
-        <v>13.05</v>
+        <v>12.75</v>
       </c>
       <c r="L6" t="n">
-        <v>11.22</v>
+        <v>11.55</v>
       </c>
       <c r="M6" t="n">
-        <v>12.72</v>
+        <v>10.72</v>
       </c>
       <c r="N6" t="n">
-        <v>12.75</v>
+        <v>9.57</v>
       </c>
       <c r="O6" t="n">
-        <v>5.42</v>
+        <v>12.98</v>
       </c>
       <c r="P6" t="n">
-        <v>13.05</v>
+        <v>11.82</v>
       </c>
       <c r="Q6" t="n">
-        <v>11.13</v>
+        <v>10.97</v>
       </c>
       <c r="R6" t="n">
-        <v>11.9</v>
+        <v>2.86</v>
       </c>
       <c r="S6" t="n">
-        <v>14.7</v>
+        <v>11.72</v>
       </c>
       <c r="T6" t="n">
-        <v>10.16</v>
+        <v>12.17</v>
       </c>
       <c r="U6" t="n">
-        <v>3.73</v>
+        <v>12.83</v>
+      </c>
+      <c r="V6" t="n">
+        <v>12.46</v>
+      </c>
+      <c r="W6" t="n">
+        <v>12.13</v>
+      </c>
+      <c r="X6" t="n">
+        <v>8.41</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>4.21</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>10.33</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>8.359999999999999</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>9.42</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>12.28</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>10.82</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>3.52</v>
       </c>
     </row>
     <row r="7">
@@ -877,65 +1077,95 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ICMO</t>
+          <t>WM</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>9.719999999999999</v>
+        <v>11.44</v>
       </c>
       <c r="D7" t="n">
-        <v>8.5</v>
+        <v>9.420000000000002</v>
       </c>
       <c r="E7" t="n">
-        <v>11.65</v>
+        <v>9.31</v>
       </c>
       <c r="F7" t="n">
-        <v>10.67</v>
+        <v>10.28</v>
       </c>
       <c r="G7" t="n">
-        <v>10</v>
+        <v>9.960000000000001</v>
       </c>
       <c r="H7" t="n">
-        <v>2.53</v>
+        <v>9.550000000000001</v>
       </c>
       <c r="I7" t="n">
-        <v>10.39</v>
+        <v>9.120000000000001</v>
       </c>
       <c r="J7" t="n">
-        <v>11.15</v>
+        <v>11.98</v>
       </c>
       <c r="K7" t="n">
-        <v>11.73</v>
+        <v>10.51</v>
       </c>
       <c r="L7" t="n">
-        <v>11.23</v>
+        <v>9.420000000000002</v>
       </c>
       <c r="M7" t="n">
-        <v>10.98</v>
+        <v>8.530000000000001</v>
       </c>
       <c r="N7" t="n">
-        <v>7.52</v>
+        <v>9.440000000000001</v>
       </c>
       <c r="O7" t="n">
-        <v>3.6</v>
+        <v>10.08</v>
       </c>
       <c r="P7" t="n">
-        <v>9.359999999999999</v>
+        <v>11.99</v>
       </c>
       <c r="Q7" t="n">
-        <v>7.879999999999999</v>
+        <v>10.2</v>
       </c>
       <c r="R7" t="n">
-        <v>8.58</v>
+        <v>3.22</v>
       </c>
       <c r="S7" t="n">
-        <v>10.9</v>
+        <v>12.49</v>
       </c>
       <c r="T7" t="n">
-        <v>10</v>
+        <v>9.81</v>
       </c>
       <c r="U7" t="n">
-        <v>3.11</v>
+        <v>9.780000000000001</v>
+      </c>
+      <c r="V7" t="n">
+        <v>8.449999999999999</v>
+      </c>
+      <c r="W7" t="n">
+        <v>9.77</v>
+      </c>
+      <c r="X7" t="n">
+        <v>11.35</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>4.61</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>11.13</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>9.07</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>9.880000000000001</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>12.29</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>8.030000000000001</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>3.19</v>
       </c>
     </row>
     <row r="8">
@@ -944,65 +1174,95 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ILRM</t>
+          <t>ILRMD</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>9.67</v>
+        <v>11.25</v>
       </c>
       <c r="D8" t="n">
-        <v>10.93</v>
+        <v>10.4</v>
       </c>
       <c r="E8" t="n">
-        <v>13.15</v>
+        <v>8.969999999999999</v>
       </c>
       <c r="F8" t="n">
-        <v>12.34</v>
+        <v>9.5</v>
       </c>
       <c r="G8" t="n">
-        <v>11.75</v>
+        <v>10.99</v>
       </c>
       <c r="H8" t="n">
-        <v>3.58</v>
+        <v>9.6</v>
       </c>
       <c r="I8" t="n">
-        <v>11.93</v>
+        <v>10.18</v>
       </c>
       <c r="J8" t="n">
-        <v>13.34</v>
+        <v>11.84</v>
       </c>
       <c r="K8" t="n">
-        <v>12.97</v>
+        <v>12.2</v>
       </c>
       <c r="L8" t="n">
-        <v>11.63</v>
+        <v>10.4</v>
       </c>
       <c r="M8" t="n">
-        <v>12.56</v>
+        <v>8.01</v>
       </c>
       <c r="N8" t="n">
-        <v>10.12</v>
+        <v>11.29</v>
       </c>
       <c r="O8" t="n">
-        <v>5.350000000000001</v>
+        <v>12.26</v>
       </c>
       <c r="P8" t="n">
-        <v>10.97</v>
+        <v>11.81</v>
       </c>
       <c r="Q8" t="n">
-        <v>10.35</v>
+        <v>11.49</v>
       </c>
       <c r="R8" t="n">
-        <v>10.75</v>
+        <v>3.95</v>
       </c>
       <c r="S8" t="n">
-        <v>12.74</v>
+        <v>11.18</v>
       </c>
       <c r="T8" t="n">
-        <v>10.08</v>
+        <v>13.29</v>
       </c>
       <c r="U8" t="n">
-        <v>3.21</v>
+        <v>12.04</v>
+      </c>
+      <c r="V8" t="n">
+        <v>10</v>
+      </c>
+      <c r="W8" t="n">
+        <v>11.94</v>
+      </c>
+      <c r="X8" t="n">
+        <v>10.84</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>5.970000000000001</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>10.67</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>11.25</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>11.07</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>12.16</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>8.640000000000001</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>2.7</v>
       </c>
     </row>
     <row r="9">
@@ -1011,65 +1271,95 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>WD</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9.050000000000001</v>
+        <v>11.24</v>
       </c>
       <c r="D9" t="n">
-        <v>9.709999999999999</v>
+        <v>9</v>
       </c>
       <c r="E9" t="n">
-        <v>10.25</v>
+        <v>8.57</v>
       </c>
       <c r="F9" t="n">
-        <v>12.46</v>
+        <v>9.859999999999999</v>
       </c>
       <c r="G9" t="n">
-        <v>10.37</v>
+        <v>9.859999999999999</v>
       </c>
       <c r="H9" t="n">
-        <v>3.33</v>
+        <v>8.610000000000001</v>
       </c>
       <c r="I9" t="n">
-        <v>13.24</v>
+        <v>8.18</v>
       </c>
       <c r="J9" t="n">
-        <v>9.649999999999999</v>
+        <v>12.1</v>
       </c>
       <c r="K9" t="n">
-        <v>9.780000000000001</v>
+        <v>10.16</v>
       </c>
       <c r="L9" t="n">
-        <v>8.700000000000001</v>
+        <v>9</v>
       </c>
       <c r="M9" t="n">
-        <v>9.880000000000001</v>
+        <v>7.67</v>
       </c>
       <c r="N9" t="n">
-        <v>11.92</v>
+        <v>10.33</v>
       </c>
       <c r="O9" t="n">
-        <v>4.8</v>
+        <v>9.73</v>
       </c>
       <c r="P9" t="n">
-        <v>11.64</v>
+        <v>11.54</v>
       </c>
       <c r="Q9" t="n">
-        <v>8.949999999999999</v>
+        <v>9.899999999999999</v>
       </c>
       <c r="R9" t="n">
-        <v>10.1</v>
+        <v>3.83</v>
       </c>
       <c r="S9" t="n">
-        <v>12.93</v>
+        <v>12.19</v>
       </c>
       <c r="T9" t="n">
-        <v>8.27</v>
+        <v>9.68</v>
       </c>
       <c r="U9" t="n">
-        <v>3.46</v>
+        <v>8.91</v>
+      </c>
+      <c r="V9" t="n">
+        <v>7.71</v>
+      </c>
+      <c r="W9" t="n">
+        <v>9.469999999999999</v>
+      </c>
+      <c r="X9" t="n">
+        <v>12.14</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>5.809999999999999</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>10.98</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>9.290000000000001</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>12.36</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>7.02</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>3.06</v>
       </c>
     </row>
     <row r="10">
@@ -1078,65 +1368,95 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ICM</t>
+          <t>FW</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8.82</v>
+        <v>10.885</v>
       </c>
       <c r="D10" t="n">
-        <v>9.709999999999999</v>
+        <v>10.525</v>
       </c>
       <c r="E10" t="n">
-        <v>11.87</v>
+        <v>7.773</v>
       </c>
       <c r="F10" t="n">
-        <v>11.19</v>
+        <v>7.463</v>
       </c>
       <c r="G10" t="n">
-        <v>10.73</v>
+        <v>8.083</v>
       </c>
       <c r="H10" t="n">
-        <v>3.15</v>
+        <v>7.533</v>
       </c>
       <c r="I10" t="n">
-        <v>10.65</v>
+        <v>10.285</v>
       </c>
       <c r="J10" t="n">
-        <v>12.22</v>
+        <v>8.443</v>
       </c>
       <c r="K10" t="n">
-        <v>11.92</v>
+        <v>10.775</v>
       </c>
       <c r="L10" t="n">
-        <v>10.55</v>
+        <v>10.525</v>
       </c>
       <c r="M10" t="n">
-        <v>11.41</v>
+        <v>12.897</v>
       </c>
       <c r="N10" t="n">
-        <v>9.029999999999999</v>
+        <v>5.942</v>
       </c>
       <c r="O10" t="n">
-        <v>4.59</v>
+        <v>8.643000000000001</v>
       </c>
       <c r="P10" t="n">
-        <v>9.950000000000001</v>
+        <v>7.472</v>
       </c>
       <c r="Q10" t="n">
-        <v>9.620000000000003</v>
+        <v>6.622</v>
       </c>
       <c r="R10" t="n">
-        <v>9.76</v>
+        <v>2.141</v>
       </c>
       <c r="S10" t="n">
-        <v>11.36</v>
+        <v>7.892</v>
       </c>
       <c r="T10" t="n">
-        <v>9.359999999999999</v>
+        <v>6.512</v>
       </c>
       <c r="U10" t="n">
-        <v>2.85</v>
+        <v>8.402999999999999</v>
+      </c>
+      <c r="V10" t="n">
+        <v>12.056</v>
+      </c>
+      <c r="W10" t="n">
+        <v>8.152999999999999</v>
+      </c>
+      <c r="X10" t="n">
+        <v>4.771000000000001</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>2.631</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>7.953</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>3.751</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>5.882</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>8.933</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>12.477</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>4.032</v>
       </c>
     </row>
     <row r="11">
@@ -1145,65 +1465,95 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>WM</t>
+          <t>ICM</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8.530000000000001</v>
+        <v>10.85</v>
       </c>
       <c r="D11" t="n">
-        <v>9.440000000000001</v>
+        <v>10.36</v>
       </c>
       <c r="E11" t="n">
-        <v>10.08</v>
+        <v>8.970000000000001</v>
       </c>
       <c r="F11" t="n">
-        <v>11.99</v>
+        <v>9</v>
       </c>
       <c r="G11" t="n">
-        <v>10.2</v>
+        <v>10.41</v>
       </c>
       <c r="H11" t="n">
-        <v>3.22</v>
+        <v>9.51</v>
       </c>
       <c r="I11" t="n">
-        <v>12.49</v>
+        <v>10.41</v>
       </c>
       <c r="J11" t="n">
-        <v>9.81</v>
+        <v>10.9</v>
       </c>
       <c r="K11" t="n">
-        <v>9.780000000000001</v>
+        <v>11.85</v>
       </c>
       <c r="L11" t="n">
-        <v>8.449999999999999</v>
+        <v>10.36</v>
       </c>
       <c r="M11" t="n">
-        <v>9.77</v>
+        <v>8.82</v>
       </c>
       <c r="N11" t="n">
-        <v>11.35</v>
+        <v>9.709999999999999</v>
       </c>
       <c r="O11" t="n">
-        <v>4.61</v>
+        <v>11.87</v>
       </c>
       <c r="P11" t="n">
-        <v>11.13</v>
+        <v>11.19</v>
       </c>
       <c r="Q11" t="n">
-        <v>9.07</v>
+        <v>10.73</v>
       </c>
       <c r="R11" t="n">
-        <v>9.880000000000001</v>
+        <v>3.15</v>
       </c>
       <c r="S11" t="n">
-        <v>12.29</v>
+        <v>10.65</v>
       </c>
       <c r="T11" t="n">
-        <v>8.030000000000001</v>
+        <v>12.22</v>
       </c>
       <c r="U11" t="n">
-        <v>3.19</v>
+        <v>11.92</v>
+      </c>
+      <c r="V11" t="n">
+        <v>10.55</v>
+      </c>
+      <c r="W11" t="n">
+        <v>11.41</v>
+      </c>
+      <c r="X11" t="n">
+        <v>9.029999999999999</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>9.950000000000001</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>9.620000000000003</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>9.76</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>11.36</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>9.359999999999999</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>2.85</v>
       </c>
     </row>
     <row r="12">
@@ -1212,65 +1562,95 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ILRMD</t>
+          <t>WB</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8.01</v>
+        <v>10.79</v>
       </c>
       <c r="D12" t="n">
-        <v>11.29</v>
+        <v>8.31</v>
       </c>
       <c r="E12" t="n">
-        <v>12.26</v>
+        <v>7.6</v>
       </c>
       <c r="F12" t="n">
-        <v>11.81</v>
+        <v>9.49</v>
       </c>
       <c r="G12" t="n">
-        <v>11.49</v>
+        <v>9.609999999999999</v>
       </c>
       <c r="H12" t="n">
-        <v>3.95</v>
+        <v>7.75</v>
       </c>
       <c r="I12" t="n">
-        <v>11.18</v>
+        <v>7.16</v>
       </c>
       <c r="J12" t="n">
-        <v>13.29</v>
+        <v>12.09</v>
       </c>
       <c r="K12" t="n">
-        <v>12.04</v>
+        <v>9.76</v>
       </c>
       <c r="L12" t="n">
-        <v>10</v>
+        <v>8.31</v>
       </c>
       <c r="M12" t="n">
-        <v>11.94</v>
+        <v>6.15</v>
       </c>
       <c r="N12" t="n">
-        <v>10.84</v>
+        <v>11.47</v>
       </c>
       <c r="O12" t="n">
-        <v>5.970000000000001</v>
+        <v>9.17</v>
       </c>
       <c r="P12" t="n">
-        <v>10.67</v>
+        <v>10.94</v>
       </c>
       <c r="Q12" t="n">
-        <v>11.25</v>
+        <v>9.76</v>
       </c>
       <c r="R12" t="n">
-        <v>11.07</v>
+        <v>4.640000000000001</v>
       </c>
       <c r="S12" t="n">
-        <v>12.16</v>
+        <v>11.38</v>
       </c>
       <c r="T12" t="n">
-        <v>8.640000000000001</v>
+        <v>10.03</v>
       </c>
       <c r="U12" t="n">
-        <v>2.7</v>
+        <v>8.02</v>
+      </c>
+      <c r="V12" t="n">
+        <v>6.42</v>
+      </c>
+      <c r="W12" t="n">
+        <v>9.17</v>
+      </c>
+      <c r="X12" t="n">
+        <v>13.24</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>7.24</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>10.79</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>10.47</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>10.91</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>12.09</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>5.71</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>2.63</v>
       </c>
     </row>
     <row r="13">
@@ -1279,65 +1659,95 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>WD</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7.67</v>
+        <v>10.68</v>
       </c>
       <c r="D13" t="n">
-        <v>10.33</v>
+        <v>10.42</v>
       </c>
       <c r="E13" t="n">
-        <v>9.73</v>
+        <v>8.23</v>
       </c>
       <c r="F13" t="n">
-        <v>11.54</v>
+        <v>7.420000000000001</v>
       </c>
       <c r="G13" t="n">
-        <v>9.899999999999999</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="H13" t="n">
-        <v>3.83</v>
+        <v>7.64</v>
       </c>
       <c r="I13" t="n">
-        <v>12.19</v>
+        <v>9.829999999999998</v>
       </c>
       <c r="J13" t="n">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="K13" t="n">
+        <v>10.77</v>
+      </c>
+      <c r="L13" t="n">
+        <v>10.42</v>
+      </c>
+      <c r="M13" t="n">
+        <v>11.58</v>
+      </c>
+      <c r="N13" t="n">
+        <v>6.93</v>
+      </c>
+      <c r="O13" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="P13" t="n">
+        <v>8.960000000000001</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>7.76</v>
+      </c>
+      <c r="R13" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="S13" t="n">
         <v>9.68</v>
       </c>
-      <c r="K13" t="n">
-        <v>8.91</v>
-      </c>
-      <c r="L13" t="n">
-        <v>7.71</v>
-      </c>
-      <c r="M13" t="n">
-        <v>9.469999999999999</v>
-      </c>
-      <c r="N13" t="n">
-        <v>12.14</v>
-      </c>
-      <c r="O13" t="n">
-        <v>5.809999999999999</v>
-      </c>
-      <c r="P13" t="n">
-        <v>10.98</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>9.290000000000001</v>
-      </c>
-      <c r="R13" t="n">
-        <v>10.2</v>
-      </c>
-      <c r="S13" t="n">
-        <v>12.36</v>
-      </c>
       <c r="T13" t="n">
-        <v>7.02</v>
+        <v>7.85</v>
       </c>
       <c r="U13" t="n">
-        <v>3.06</v>
+        <v>9.609999999999999</v>
+      </c>
+      <c r="V13" t="n">
+        <v>11.92</v>
+      </c>
+      <c r="W13" t="n">
+        <v>9.26</v>
+      </c>
+      <c r="X13" t="n">
+        <v>5.69</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>3.05</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>8.359999999999999</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>4.119999999999999</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>6.47</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>10.24</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>10.86</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>3.87</v>
       </c>
     </row>
     <row r="14">
@@ -1346,65 +1756,95 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ICMD</t>
+          <t>ICMO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>7.4</v>
+        <v>10.65</v>
       </c>
       <c r="D14" t="n">
-        <v>10.1</v>
+        <v>10.45</v>
       </c>
       <c r="E14" t="n">
-        <v>11.19</v>
+        <v>8.959999999999999</v>
       </c>
       <c r="F14" t="n">
-        <v>10.81</v>
+        <v>8.49</v>
       </c>
       <c r="G14" t="n">
-        <v>10.56</v>
+        <v>10.03</v>
       </c>
       <c r="H14" t="n">
-        <v>3.489999999999999</v>
+        <v>9.239999999999998</v>
       </c>
       <c r="I14" t="n">
-        <v>10.11</v>
+        <v>10.53</v>
       </c>
       <c r="J14" t="n">
-        <v>12.23</v>
+        <v>10.23</v>
       </c>
       <c r="K14" t="n">
-        <v>11.17</v>
+        <v>11.6</v>
       </c>
       <c r="L14" t="n">
-        <v>9.19</v>
+        <v>10.45</v>
       </c>
       <c r="M14" t="n">
-        <v>10.94</v>
+        <v>9.719999999999999</v>
       </c>
       <c r="N14" t="n">
-        <v>9.720000000000001</v>
+        <v>8.5</v>
       </c>
       <c r="O14" t="n">
-        <v>5.18</v>
+        <v>11.65</v>
       </c>
       <c r="P14" t="n">
-        <v>9.739999999999998</v>
+        <v>10.67</v>
       </c>
       <c r="Q14" t="n">
-        <v>10.4</v>
+        <v>10</v>
       </c>
       <c r="R14" t="n">
-        <v>10.08</v>
+        <v>2.53</v>
       </c>
       <c r="S14" t="n">
-        <v>10.96</v>
+        <v>10.39</v>
       </c>
       <c r="T14" t="n">
-        <v>8.1</v>
+        <v>11.15</v>
       </c>
       <c r="U14" t="n">
-        <v>2.43</v>
+        <v>11.73</v>
+      </c>
+      <c r="V14" t="n">
+        <v>11.23</v>
+      </c>
+      <c r="W14" t="n">
+        <v>10.98</v>
+      </c>
+      <c r="X14" t="n">
+        <v>7.52</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>9.359999999999999</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>7.879999999999999</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>8.58</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>3.11</v>
       </c>
     </row>
     <row r="15">
@@ -1413,65 +1853,95 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>WBO</t>
+          <t>WBM</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6.43</v>
+        <v>10.59</v>
       </c>
       <c r="D15" t="n">
-        <v>10.5</v>
+        <v>8.359999999999999</v>
       </c>
       <c r="E15" t="n">
-        <v>8.720000000000001</v>
+        <v>7.3</v>
       </c>
       <c r="F15" t="n">
+        <v>9.140000000000001</v>
+      </c>
+      <c r="G15" t="n">
+        <v>9.81</v>
+      </c>
+      <c r="H15" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="I15" t="n">
+        <v>7.109999999999999</v>
+      </c>
+      <c r="J15" t="n">
+        <v>12.04</v>
+      </c>
+      <c r="K15" t="n">
+        <v>10.01</v>
+      </c>
+      <c r="L15" t="n">
+        <v>8.359999999999999</v>
+      </c>
+      <c r="M15" t="n">
+        <v>5.65</v>
+      </c>
+      <c r="N15" t="n">
+        <v>12.12</v>
+      </c>
+      <c r="O15" t="n">
+        <v>9.619999999999999</v>
+      </c>
+      <c r="P15" t="n">
         <v>10.79</v>
       </c>
-      <c r="G15" t="n">
-        <v>9.41</v>
-      </c>
-      <c r="H15" t="n">
-        <v>4.16</v>
-      </c>
-      <c r="I15" t="n">
-        <v>11.28</v>
-      </c>
-      <c r="J15" t="n">
-        <v>9.32</v>
-      </c>
-      <c r="K15" t="n">
-        <v>7.83</v>
-      </c>
-      <c r="L15" t="n">
-        <v>6.34</v>
-      </c>
-      <c r="M15" t="n">
-        <v>8.720000000000001</v>
-      </c>
-      <c r="N15" t="n">
-        <v>12.57</v>
-      </c>
-      <c r="O15" t="n">
-        <v>6.34</v>
-      </c>
-      <c r="P15" t="n">
+      <c r="Q15" t="n">
+        <v>10.01</v>
+      </c>
+      <c r="R15" t="n">
+        <v>4.94</v>
+      </c>
+      <c r="S15" t="n">
+        <v>10.98</v>
+      </c>
+      <c r="T15" t="n">
+        <v>10.88</v>
+      </c>
+      <c r="U15" t="n">
+        <v>8.370000000000001</v>
+      </c>
+      <c r="V15" t="n">
+        <v>6.52</v>
+      </c>
+      <c r="W15" t="n">
+        <v>9.619999999999999</v>
+      </c>
+      <c r="X15" t="n">
+        <v>13.29</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>7.84</v>
+      </c>
+      <c r="Z15" t="n">
         <v>10.59</v>
       </c>
-      <c r="Q15" t="n">
-        <v>9.809999999999999</v>
-      </c>
-      <c r="R15" t="n">
-        <v>10.3</v>
-      </c>
-      <c r="S15" t="n">
-        <v>11.68</v>
-      </c>
-      <c r="T15" t="n">
-        <v>5.94</v>
-      </c>
-      <c r="U15" t="n">
-        <v>2.67</v>
+      <c r="AA15" t="n">
+        <v>11.07</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>11.26</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>12.04</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>5.46</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>2.43</v>
       </c>
     </row>
     <row r="16">
@@ -1480,65 +1950,95 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>WB</t>
+          <t>WBO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>6.15</v>
+        <v>10.59</v>
       </c>
       <c r="D16" t="n">
-        <v>11.47</v>
+        <v>8.119999999999999</v>
       </c>
       <c r="E16" t="n">
-        <v>9.17</v>
+        <v>7.719999999999999</v>
       </c>
       <c r="F16" t="n">
-        <v>10.94</v>
+        <v>9.5</v>
       </c>
       <c r="G16" t="n">
-        <v>9.76</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="H16" t="n">
-        <v>4.640000000000001</v>
+        <v>7.92</v>
       </c>
       <c r="I16" t="n">
-        <v>11.38</v>
+        <v>7.23</v>
       </c>
       <c r="J16" t="n">
-        <v>10.03</v>
+        <v>11.68</v>
       </c>
       <c r="K16" t="n">
-        <v>8.02</v>
+        <v>9.41</v>
       </c>
       <c r="L16" t="n">
-        <v>6.42</v>
+        <v>8.119999999999999</v>
       </c>
       <c r="M16" t="n">
-        <v>9.17</v>
+        <v>6.43</v>
       </c>
       <c r="N16" t="n">
-        <v>13.24</v>
+        <v>10.5</v>
       </c>
       <c r="O16" t="n">
-        <v>7.24</v>
+        <v>8.720000000000001</v>
       </c>
       <c r="P16" t="n">
         <v>10.79</v>
       </c>
       <c r="Q16" t="n">
-        <v>10.47</v>
+        <v>9.41</v>
       </c>
       <c r="R16" t="n">
-        <v>10.91</v>
+        <v>4.16</v>
       </c>
       <c r="S16" t="n">
-        <v>12.09</v>
+        <v>11.28</v>
       </c>
       <c r="T16" t="n">
-        <v>5.71</v>
+        <v>9.32</v>
       </c>
       <c r="U16" t="n">
-        <v>2.63</v>
+        <v>7.83</v>
+      </c>
+      <c r="V16" t="n">
+        <v>6.34</v>
+      </c>
+      <c r="W16" t="n">
+        <v>8.720000000000001</v>
+      </c>
+      <c r="X16" t="n">
+        <v>12.57</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>6.34</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>10.59</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>9.809999999999999</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>11.68</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>5.94</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>2.67</v>
       </c>
     </row>
     <row r="17">
@@ -1547,65 +2047,95 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>CDO</t>
+          <t>WBD</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>6.12</v>
+        <v>10.35</v>
       </c>
       <c r="D17" t="n">
-        <v>8.32</v>
+        <v>8.02</v>
       </c>
       <c r="E17" t="n">
-        <v>8.58</v>
+        <v>7.04</v>
       </c>
       <c r="F17" t="n">
-        <v>9.780000000000001</v>
+        <v>8.92</v>
       </c>
       <c r="G17" t="n">
-        <v>8.98</v>
+        <v>9.450000000000001</v>
       </c>
       <c r="H17" t="n">
-        <v>2.93</v>
+        <v>7.140000000000001</v>
       </c>
       <c r="I17" t="n">
-        <v>9.450000000000001</v>
+        <v>6.69</v>
       </c>
       <c r="J17" t="n">
-        <v>9.510000000000002</v>
+        <v>11.78</v>
       </c>
       <c r="K17" t="n">
-        <v>8.710000000000001</v>
+        <v>9.550000000000001</v>
       </c>
       <c r="L17" t="n">
-        <v>6.65</v>
+        <v>8.02</v>
       </c>
       <c r="M17" t="n">
-        <v>8.58</v>
+        <v>5.51</v>
       </c>
       <c r="N17" t="n">
-        <v>9.52</v>
+        <v>11.76</v>
       </c>
       <c r="O17" t="n">
-        <v>4.13</v>
+        <v>9.1</v>
       </c>
       <c r="P17" t="n">
-        <v>9.050000000000001</v>
+        <v>10.45</v>
       </c>
       <c r="Q17" t="n">
-        <v>9.18</v>
+        <v>9.550000000000001</v>
       </c>
       <c r="R17" t="n">
-        <v>8.85</v>
+        <v>4.84</v>
       </c>
       <c r="S17" t="n">
-        <v>9.65</v>
+        <v>10.8</v>
       </c>
       <c r="T17" t="n">
-        <v>6.449999999999999</v>
+        <v>10.18</v>
       </c>
       <c r="U17" t="n">
-        <v>2.13</v>
+        <v>7.77</v>
+      </c>
+      <c r="V17" t="n">
+        <v>6.140000000000001</v>
+      </c>
+      <c r="W17" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="X17" t="n">
+        <v>13.11</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>10.35</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>10.53</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>10.88</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>11.78</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>5.16</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>2.43</v>
       </c>
     </row>
     <row r="18">
@@ -1614,64 +2144,94 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>WBM</t>
+          <t>ICMD</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>5.65</v>
+        <v>10.25</v>
       </c>
       <c r="D18" t="n">
-        <v>12.12</v>
+        <v>9.529999999999999</v>
       </c>
       <c r="E18" t="n">
-        <v>9.619999999999999</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="F18" t="n">
-        <v>10.79</v>
+        <v>8.77</v>
       </c>
       <c r="G18" t="n">
-        <v>10.01</v>
+        <v>9.989999999999998</v>
       </c>
       <c r="H18" t="n">
-        <v>4.94</v>
+        <v>9</v>
       </c>
       <c r="I18" t="n">
-        <v>10.98</v>
+        <v>9.509999999999998</v>
       </c>
       <c r="J18" t="n">
-        <v>10.88</v>
+        <v>10.71</v>
       </c>
       <c r="K18" t="n">
-        <v>8.370000000000001</v>
+        <v>11.2</v>
       </c>
       <c r="L18" t="n">
-        <v>6.52</v>
+        <v>9.529999999999999</v>
       </c>
       <c r="M18" t="n">
-        <v>9.619999999999999</v>
+        <v>7.4</v>
       </c>
       <c r="N18" t="n">
-        <v>13.29</v>
+        <v>10.1</v>
       </c>
       <c r="O18" t="n">
-        <v>7.84</v>
+        <v>11.19</v>
       </c>
       <c r="P18" t="n">
-        <v>10.59</v>
+        <v>10.81</v>
       </c>
       <c r="Q18" t="n">
-        <v>11.07</v>
+        <v>10.56</v>
       </c>
       <c r="R18" t="n">
-        <v>11.26</v>
+        <v>3.489999999999999</v>
       </c>
       <c r="S18" t="n">
-        <v>12.04</v>
+        <v>10.11</v>
       </c>
       <c r="T18" t="n">
-        <v>5.46</v>
+        <v>12.23</v>
       </c>
       <c r="U18" t="n">
+        <v>11.17</v>
+      </c>
+      <c r="V18" t="n">
+        <v>9.19</v>
+      </c>
+      <c r="W18" t="n">
+        <v>10.94</v>
+      </c>
+      <c r="X18" t="n">
+        <v>9.720000000000001</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>5.18</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>9.739999999999998</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>10.08</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>10.96</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="AE18" t="n">
         <v>2.43</v>
       </c>
     </row>
@@ -1681,65 +2241,95 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>WBD</t>
+          <t>CDW</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>5.51</v>
+        <v>9.710000000000001</v>
       </c>
       <c r="D19" t="n">
-        <v>11.76</v>
+        <v>7.71</v>
       </c>
       <c r="E19" t="n">
-        <v>9.1</v>
+        <v>6.49</v>
       </c>
       <c r="F19" t="n">
+        <v>8.23</v>
+      </c>
+      <c r="G19" t="n">
+        <v>9.190000000000001</v>
+      </c>
+      <c r="H19" t="n">
+        <v>6.64</v>
+      </c>
+      <c r="I19" t="n">
+        <v>6.38</v>
+      </c>
+      <c r="J19" t="n">
+        <v>11.19</v>
+      </c>
+      <c r="K19" t="n">
+        <v>9.34</v>
+      </c>
+      <c r="L19" t="n">
+        <v>7.71</v>
+      </c>
+      <c r="M19" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="N19" t="n">
+        <v>11.74</v>
+      </c>
+      <c r="O19" t="n">
+        <v>9.08</v>
+      </c>
+      <c r="P19" t="n">
+        <v>9.860000000000001</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>9.34</v>
+      </c>
+      <c r="R19" t="n">
+        <v>4.850000000000001</v>
+      </c>
+      <c r="S19" t="n">
+        <v>9.970000000000001</v>
+      </c>
+      <c r="T19" t="n">
         <v>10.45</v>
       </c>
-      <c r="G19" t="n">
-        <v>9.550000000000001</v>
-      </c>
-      <c r="H19" t="n">
-        <v>4.84</v>
-      </c>
-      <c r="I19" t="n">
-        <v>10.8</v>
-      </c>
-      <c r="J19" t="n">
-        <v>10.18</v>
-      </c>
-      <c r="K19" t="n">
-        <v>7.77</v>
-      </c>
-      <c r="L19" t="n">
-        <v>6.140000000000001</v>
-      </c>
-      <c r="M19" t="n">
-        <v>9.1</v>
-      </c>
-      <c r="N19" t="n">
-        <v>13.11</v>
-      </c>
-      <c r="O19" t="n">
-        <v>7.7</v>
-      </c>
-      <c r="P19" t="n">
-        <v>10.35</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>10.53</v>
-      </c>
-      <c r="R19" t="n">
-        <v>10.88</v>
-      </c>
-      <c r="S19" t="n">
-        <v>11.78</v>
-      </c>
-      <c r="T19" t="n">
-        <v>5.16</v>
-      </c>
       <c r="U19" t="n">
-        <v>2.43</v>
+        <v>7.75</v>
+      </c>
+      <c r="V19" t="n">
+        <v>5.970000000000001</v>
+      </c>
+      <c r="W19" t="n">
+        <v>9.08</v>
+      </c>
+      <c r="X19" t="n">
+        <v>12.52</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>7.81</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>9.710000000000001</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>10.56</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>10.67</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>11.19</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>2.15</v>
       </c>
     </row>
     <row r="20">
@@ -1748,65 +2338,95 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>CDW</t>
+          <t>CDO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>4.86</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="D20" t="n">
-        <v>11.74</v>
+        <v>7.65</v>
       </c>
       <c r="E20" t="n">
-        <v>9.08</v>
+        <v>7.45</v>
       </c>
       <c r="F20" t="n">
-        <v>9.860000000000001</v>
+        <v>8.450000000000001</v>
       </c>
       <c r="G20" t="n">
-        <v>9.34</v>
+        <v>8.25</v>
       </c>
       <c r="H20" t="n">
-        <v>4.850000000000001</v>
+        <v>8.18</v>
       </c>
       <c r="I20" t="n">
-        <v>9.970000000000001</v>
+        <v>7.779999999999999</v>
       </c>
       <c r="J20" t="n">
-        <v>10.45</v>
+        <v>9.65</v>
       </c>
       <c r="K20" t="n">
-        <v>7.75</v>
+        <v>8.98</v>
       </c>
       <c r="L20" t="n">
-        <v>5.970000000000001</v>
+        <v>7.65</v>
       </c>
       <c r="M20" t="n">
-        <v>9.08</v>
+        <v>6.12</v>
       </c>
       <c r="N20" t="n">
-        <v>12.52</v>
+        <v>8.32</v>
       </c>
       <c r="O20" t="n">
-        <v>7.81</v>
+        <v>8.58</v>
       </c>
       <c r="P20" t="n">
-        <v>9.710000000000001</v>
+        <v>9.780000000000001</v>
       </c>
       <c r="Q20" t="n">
-        <v>10.56</v>
+        <v>8.98</v>
       </c>
       <c r="R20" t="n">
-        <v>10.67</v>
+        <v>2.93</v>
       </c>
       <c r="S20" t="n">
-        <v>11.19</v>
+        <v>9.450000000000001</v>
       </c>
       <c r="T20" t="n">
-        <v>4.75</v>
+        <v>9.510000000000002</v>
       </c>
       <c r="U20" t="n">
-        <v>2.15</v>
+        <v>8.710000000000001</v>
+      </c>
+      <c r="V20" t="n">
+        <v>6.65</v>
+      </c>
+      <c r="W20" t="n">
+        <v>8.58</v>
+      </c>
+      <c r="X20" t="n">
+        <v>9.52</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>9.050000000000001</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>9.18</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>8.85</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>9.65</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>6.449999999999999</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>2.13</v>
       </c>
     </row>
     <row r="21">
@@ -1815,65 +2435,95 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>WO</t>
+          <t>CLRD</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>4.5</v>
+        <v>8.85</v>
       </c>
       <c r="D21" t="n">
-        <v>5.630000000000001</v>
+        <v>7.33</v>
       </c>
       <c r="E21" t="n">
-        <v>6.37</v>
+        <v>5.81</v>
       </c>
       <c r="F21" t="n">
-        <v>6.25</v>
+        <v>7.33</v>
       </c>
       <c r="G21" t="n">
-        <v>5.629999999999999</v>
+        <v>8.85</v>
       </c>
       <c r="H21" t="n">
-        <v>1.87</v>
+        <v>6.06</v>
       </c>
       <c r="I21" t="n">
-        <v>6.47</v>
+        <v>6.06</v>
       </c>
       <c r="J21" t="n">
-        <v>6.08</v>
+        <v>10.37</v>
       </c>
       <c r="K21" t="n">
-        <v>5.9</v>
+        <v>9.1</v>
       </c>
       <c r="L21" t="n">
-        <v>5.37</v>
+        <v>7.33</v>
       </c>
       <c r="M21" t="n">
-        <v>5.95</v>
+        <v>4.04</v>
       </c>
       <c r="N21" t="n">
-        <v>5.51</v>
+        <v>11.64</v>
       </c>
       <c r="O21" t="n">
-        <v>2.989999999999999</v>
+        <v>9.1</v>
       </c>
       <c r="P21" t="n">
-        <v>5.529999999999999</v>
+        <v>9.1</v>
       </c>
       <c r="Q21" t="n">
-        <v>4.62</v>
+        <v>9.1</v>
       </c>
       <c r="R21" t="n">
-        <v>5.26</v>
+        <v>4.81</v>
       </c>
       <c r="S21" t="n">
-        <v>6.72</v>
+        <v>8.85</v>
       </c>
       <c r="T21" t="n">
-        <v>4.28</v>
+        <v>10.87</v>
       </c>
       <c r="U21" t="n">
-        <v>1.69</v>
+        <v>7.83</v>
+      </c>
+      <c r="V21" t="n">
+        <v>5.81</v>
+      </c>
+      <c r="W21" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="X21" t="n">
+        <v>11.64</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>7.85</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>8.85</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>10.62</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>10.37</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>10.37</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>1.77</v>
       </c>
     </row>
     <row r="22">
@@ -1882,65 +2532,95 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>CLRD</t>
+          <t>CCD</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>4.04</v>
+        <v>7.55</v>
       </c>
       <c r="D22" t="n">
-        <v>11.64</v>
+        <v>6.29</v>
       </c>
       <c r="E22" t="n">
-        <v>9.1</v>
+        <v>5.03</v>
       </c>
       <c r="F22" t="n">
-        <v>9.1</v>
+        <v>6.29</v>
       </c>
       <c r="G22" t="n">
-        <v>9.1</v>
+        <v>7.55</v>
       </c>
       <c r="H22" t="n">
-        <v>4.81</v>
+        <v>5.28</v>
       </c>
       <c r="I22" t="n">
-        <v>8.85</v>
+        <v>5.28</v>
       </c>
       <c r="J22" t="n">
-        <v>10.87</v>
+        <v>8.81</v>
       </c>
       <c r="K22" t="n">
-        <v>7.83</v>
+        <v>7.8</v>
       </c>
       <c r="L22" t="n">
-        <v>5.81</v>
+        <v>6.29</v>
       </c>
       <c r="M22" t="n">
-        <v>9.1</v>
+        <v>3.52</v>
       </c>
       <c r="N22" t="n">
-        <v>11.64</v>
+        <v>9.82</v>
       </c>
       <c r="O22" t="n">
-        <v>7.85</v>
+        <v>7.8</v>
       </c>
       <c r="P22" t="n">
-        <v>8.85</v>
+        <v>7.8</v>
       </c>
       <c r="Q22" t="n">
-        <v>10.62</v>
+        <v>7.8</v>
       </c>
       <c r="R22" t="n">
-        <v>10.37</v>
+        <v>4.03</v>
       </c>
       <c r="S22" t="n">
-        <v>10.37</v>
+        <v>7.55</v>
       </c>
       <c r="T22" t="n">
-        <v>4.29</v>
+        <v>9.31</v>
       </c>
       <c r="U22" t="n">
-        <v>1.77</v>
+        <v>6.79</v>
+      </c>
+      <c r="V22" t="n">
+        <v>5.03</v>
+      </c>
+      <c r="W22" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="X22" t="n">
+        <v>9.82</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>6.55</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>7.55</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>9.06</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>8.81</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>8.81</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>1.51</v>
       </c>
     </row>
     <row r="23">
@@ -1949,65 +2629,95 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>CCD</t>
+          <t>WO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3.52</v>
+        <v>5.95</v>
       </c>
       <c r="D23" t="n">
-        <v>9.82</v>
+        <v>5.4</v>
       </c>
       <c r="E23" t="n">
-        <v>7.8</v>
+        <v>4.73</v>
       </c>
       <c r="F23" t="n">
-        <v>7.8</v>
+        <v>4.76</v>
       </c>
       <c r="G23" t="n">
-        <v>7.8</v>
+        <v>5.75</v>
       </c>
       <c r="H23" t="n">
-        <v>4.03</v>
+        <v>4.609999999999999</v>
       </c>
       <c r="I23" t="n">
-        <v>7.55</v>
+        <v>4.93</v>
       </c>
       <c r="J23" t="n">
-        <v>9.31</v>
+        <v>6.300000000000001</v>
       </c>
       <c r="K23" t="n">
-        <v>6.79</v>
+        <v>6.050000000000001</v>
       </c>
       <c r="L23" t="n">
-        <v>5.03</v>
+        <v>5.4</v>
       </c>
       <c r="M23" t="n">
-        <v>7.8</v>
+        <v>4.5</v>
       </c>
       <c r="N23" t="n">
-        <v>9.82</v>
+        <v>5.630000000000001</v>
       </c>
       <c r="O23" t="n">
-        <v>6.55</v>
+        <v>6.37</v>
       </c>
       <c r="P23" t="n">
-        <v>7.55</v>
+        <v>6.25</v>
       </c>
       <c r="Q23" t="n">
-        <v>9.06</v>
+        <v>5.629999999999999</v>
       </c>
       <c r="R23" t="n">
-        <v>8.81</v>
+        <v>1.87</v>
       </c>
       <c r="S23" t="n">
-        <v>8.81</v>
+        <v>6.47</v>
       </c>
       <c r="T23" t="n">
-        <v>3.77</v>
+        <v>6.08</v>
       </c>
       <c r="U23" t="n">
-        <v>1.51</v>
+        <v>5.9</v>
+      </c>
+      <c r="V23" t="n">
+        <v>5.37</v>
+      </c>
+      <c r="W23" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="X23" t="n">
+        <v>5.51</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>2.989999999999999</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>5.529999999999999</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>4.62</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>6.72</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>4.28</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>1.69</v>
       </c>
     </row>
     <row r="24">
@@ -2020,60 +2730,90 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2.68</v>
+        <v>4.48</v>
       </c>
       <c r="D24" t="n">
-        <v>5.68</v>
+        <v>3.88</v>
       </c>
       <c r="E24" t="n">
-        <v>4.48</v>
+        <v>3.28</v>
       </c>
       <c r="F24" t="n">
-        <v>4.48</v>
+        <v>3.88</v>
       </c>
       <c r="G24" t="n">
         <v>4.48</v>
       </c>
       <c r="H24" t="n">
-        <v>10.68</v>
+        <v>3.28</v>
       </c>
       <c r="I24" t="n">
-        <v>4.48</v>
+        <v>3.28</v>
       </c>
       <c r="J24" t="n">
         <v>5.08</v>
       </c>
       <c r="K24" t="n">
+        <v>4.48</v>
+      </c>
+      <c r="L24" t="n">
         <v>3.88</v>
       </c>
-      <c r="L24" t="n">
-        <v>3.28</v>
-      </c>
       <c r="M24" t="n">
-        <v>5.96</v>
+        <v>2.68</v>
       </c>
       <c r="N24" t="n">
         <v>5.68</v>
       </c>
       <c r="O24" t="n">
-        <v>11.88</v>
+        <v>4.48</v>
       </c>
       <c r="P24" t="n">
         <v>4.48</v>
       </c>
       <c r="Q24" t="n">
+        <v>4.48</v>
+      </c>
+      <c r="R24" t="n">
+        <v>10.68</v>
+      </c>
+      <c r="S24" t="n">
+        <v>4.48</v>
+      </c>
+      <c r="T24" t="n">
         <v>5.08</v>
       </c>
-      <c r="R24" t="n">
+      <c r="U24" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="V24" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="W24" t="n">
+        <v>5.96</v>
+      </c>
+      <c r="X24" t="n">
+        <v>5.68</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>11.88</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>4.48</v>
+      </c>
+      <c r="AA24" t="n">
         <v>5.08</v>
       </c>
-      <c r="S24" t="n">
+      <c r="AB24" t="n">
+        <v>5.08</v>
+      </c>
+      <c r="AC24" t="n">
         <v>6.56</v>
       </c>
-      <c r="T24" t="n">
+      <c r="AD24" t="n">
         <v>2.68</v>
       </c>
-      <c r="U24" t="n">
+      <c r="AE24" t="n">
         <v>3.56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added plotting of statistics
</commit_message>
<xml_diff>
--- a/Player_Analysis/Team_Results.xlsx
+++ b/Player_Analysis/Team_Results.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE24"/>
+  <dimension ref="A1:AD24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,65 +522,60 @@
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Pacífico Alpízar</t>
+          <t>Cole Frampton</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Cole Frampton</t>
+          <t>Steven Shotwell</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Steven Shotwell</t>
+          <t>Roy Belcher</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Roy Belcher</t>
+          <t>Austin Liner</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Austin Liner</t>
+          <t>Israel Vernon</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Israel Vernon</t>
+          <t>Jack McCray</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Jack McCray</t>
+          <t>Tom Hayden</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>Tom Hayden</t>
+          <t>Demetrius Machen</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>Demetrius Machen</t>
+          <t>Jared Vernon</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Jared Vernon</t>
+          <t>Joey Cartwright</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>Joey Cartwright</t>
+          <t>Mazen Dergham</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>Mazen Dergham</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Rogelio Nakamura</t>
         </is>
@@ -623,7 +618,7 @@
         <v>13.31</v>
       </c>
       <c r="L2" t="n">
-        <v>11.84</v>
+        <v>12.43</v>
       </c>
       <c r="M2" t="n">
         <v>10.39</v>
@@ -644,43 +639,40 @@
         <v>3.74</v>
       </c>
       <c r="S2" t="n">
-        <v>14.72</v>
+        <v>13.06</v>
       </c>
       <c r="T2" t="n">
-        <v>13.06</v>
+        <v>13.05</v>
       </c>
       <c r="U2" t="n">
+        <v>11.22</v>
+      </c>
+      <c r="V2" t="n">
+        <v>12.72</v>
+      </c>
+      <c r="W2" t="n">
+        <v>12.75</v>
+      </c>
+      <c r="X2" t="n">
+        <v>5.42</v>
+      </c>
+      <c r="Y2" t="n">
         <v>13.05</v>
       </c>
-      <c r="V2" t="n">
-        <v>11.22</v>
-      </c>
-      <c r="W2" t="n">
-        <v>12.72</v>
-      </c>
-      <c r="X2" t="n">
-        <v>12.75</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>5.42</v>
-      </c>
       <c r="Z2" t="n">
-        <v>13.05</v>
+        <v>11.13</v>
       </c>
       <c r="AA2" t="n">
-        <v>11.13</v>
+        <v>11.9</v>
       </c>
       <c r="AB2" t="n">
-        <v>11.9</v>
+        <v>14.7</v>
       </c>
       <c r="AC2" t="n">
-        <v>14.7</v>
+        <v>10.16</v>
       </c>
       <c r="AD2" t="n">
-        <v>10.16</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>3.73</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="3">
@@ -720,7 +712,7 @@
         <v>11.51</v>
       </c>
       <c r="L3" t="n">
-        <v>11.36</v>
+        <v>12</v>
       </c>
       <c r="M3" t="n">
         <v>14.19</v>
@@ -741,43 +733,40 @@
         <v>2.4</v>
       </c>
       <c r="S3" t="n">
-        <v>10.21</v>
+        <v>6.43</v>
       </c>
       <c r="T3" t="n">
-        <v>6.43</v>
+        <v>8.68</v>
       </c>
       <c r="U3" t="n">
-        <v>8.68</v>
+        <v>12.33</v>
       </c>
       <c r="V3" t="n">
-        <v>12.33</v>
+        <v>8.530000000000001</v>
       </c>
       <c r="W3" t="n">
-        <v>8.530000000000001</v>
+        <v>6.93</v>
       </c>
       <c r="X3" t="n">
-        <v>6.93</v>
+        <v>2.84</v>
       </c>
       <c r="Y3" t="n">
+        <v>9.859999999999999</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>6.970000000000001</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>10.74</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>13.26</v>
+      </c>
+      <c r="AD3" t="n">
         <v>2.84</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>9.859999999999999</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>4.43</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>6.970000000000001</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>10.74</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>13.26</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>4.649999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -817,7 +806,7 @@
         <v>10.74</v>
       </c>
       <c r="L4" t="n">
-        <v>9.740000000000002</v>
+        <v>10.6</v>
       </c>
       <c r="M4" t="n">
         <v>9.050000000000001</v>
@@ -838,43 +827,40 @@
         <v>3.33</v>
       </c>
       <c r="S4" t="n">
-        <v>13.24</v>
+        <v>9.649999999999999</v>
       </c>
       <c r="T4" t="n">
-        <v>9.649999999999999</v>
+        <v>9.780000000000001</v>
       </c>
       <c r="U4" t="n">
-        <v>9.780000000000001</v>
+        <v>8.700000000000001</v>
       </c>
       <c r="V4" t="n">
-        <v>8.700000000000001</v>
+        <v>9.880000000000001</v>
       </c>
       <c r="W4" t="n">
-        <v>9.880000000000001</v>
+        <v>11.92</v>
       </c>
       <c r="X4" t="n">
-        <v>11.92</v>
+        <v>4.8</v>
       </c>
       <c r="Y4" t="n">
-        <v>4.8</v>
+        <v>11.64</v>
       </c>
       <c r="Z4" t="n">
-        <v>11.64</v>
+        <v>8.949999999999999</v>
       </c>
       <c r="AA4" t="n">
-        <v>8.949999999999999</v>
+        <v>10.1</v>
       </c>
       <c r="AB4" t="n">
-        <v>10.1</v>
+        <v>12.93</v>
       </c>
       <c r="AC4" t="n">
-        <v>12.93</v>
+        <v>8.27</v>
       </c>
       <c r="AD4" t="n">
-        <v>8.27</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>3.46</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="5">
@@ -935,43 +921,40 @@
         <v>3.58</v>
       </c>
       <c r="S5" t="n">
-        <v>11.93</v>
+        <v>13.34</v>
       </c>
       <c r="T5" t="n">
-        <v>13.34</v>
+        <v>12.97</v>
       </c>
       <c r="U5" t="n">
-        <v>12.97</v>
+        <v>11.63</v>
       </c>
       <c r="V5" t="n">
-        <v>11.63</v>
+        <v>12.56</v>
       </c>
       <c r="W5" t="n">
-        <v>12.56</v>
+        <v>10.12</v>
       </c>
       <c r="X5" t="n">
-        <v>10.12</v>
+        <v>5.350000000000001</v>
       </c>
       <c r="Y5" t="n">
-        <v>5.350000000000001</v>
+        <v>10.97</v>
       </c>
       <c r="Z5" t="n">
-        <v>10.97</v>
+        <v>10.35</v>
       </c>
       <c r="AA5" t="n">
-        <v>10.35</v>
+        <v>10.75</v>
       </c>
       <c r="AB5" t="n">
-        <v>10.75</v>
+        <v>12.74</v>
       </c>
       <c r="AC5" t="n">
-        <v>12.74</v>
+        <v>10.08</v>
       </c>
       <c r="AD5" t="n">
-        <v>10.08</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>3.21</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="6">
@@ -1032,43 +1015,40 @@
         <v>2.86</v>
       </c>
       <c r="S6" t="n">
-        <v>11.72</v>
+        <v>12.17</v>
       </c>
       <c r="T6" t="n">
-        <v>12.17</v>
+        <v>12.83</v>
       </c>
       <c r="U6" t="n">
-        <v>12.83</v>
+        <v>12.46</v>
       </c>
       <c r="V6" t="n">
-        <v>12.46</v>
+        <v>12.13</v>
       </c>
       <c r="W6" t="n">
-        <v>12.13</v>
+        <v>8.41</v>
       </c>
       <c r="X6" t="n">
-        <v>8.41</v>
+        <v>4.21</v>
       </c>
       <c r="Y6" t="n">
-        <v>4.21</v>
+        <v>10.33</v>
       </c>
       <c r="Z6" t="n">
-        <v>10.33</v>
+        <v>8.359999999999999</v>
       </c>
       <c r="AA6" t="n">
-        <v>8.359999999999999</v>
+        <v>9.42</v>
       </c>
       <c r="AB6" t="n">
-        <v>9.42</v>
+        <v>12.28</v>
       </c>
       <c r="AC6" t="n">
-        <v>12.28</v>
+        <v>10.82</v>
       </c>
       <c r="AD6" t="n">
-        <v>10.82</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>3.52</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="7">
@@ -1108,7 +1088,7 @@
         <v>10.51</v>
       </c>
       <c r="L7" t="n">
-        <v>9.420000000000002</v>
+        <v>10.16</v>
       </c>
       <c r="M7" t="n">
         <v>8.530000000000001</v>
@@ -1129,43 +1109,40 @@
         <v>3.22</v>
       </c>
       <c r="S7" t="n">
-        <v>12.49</v>
+        <v>9.81</v>
       </c>
       <c r="T7" t="n">
-        <v>9.81</v>
+        <v>9.780000000000001</v>
       </c>
       <c r="U7" t="n">
-        <v>9.780000000000001</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="V7" t="n">
-        <v>8.449999999999999</v>
+        <v>9.77</v>
       </c>
       <c r="W7" t="n">
-        <v>9.77</v>
+        <v>11.35</v>
       </c>
       <c r="X7" t="n">
-        <v>11.35</v>
+        <v>4.61</v>
       </c>
       <c r="Y7" t="n">
-        <v>4.61</v>
+        <v>11.13</v>
       </c>
       <c r="Z7" t="n">
-        <v>11.13</v>
+        <v>9.07</v>
       </c>
       <c r="AA7" t="n">
-        <v>9.07</v>
+        <v>9.880000000000001</v>
       </c>
       <c r="AB7" t="n">
-        <v>9.880000000000001</v>
+        <v>12.29</v>
       </c>
       <c r="AC7" t="n">
-        <v>12.29</v>
+        <v>8.030000000000001</v>
       </c>
       <c r="AD7" t="n">
-        <v>8.030000000000001</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>3.19</v>
+        <v>2.45</v>
       </c>
     </row>
     <row r="8">
@@ -1226,43 +1203,40 @@
         <v>3.95</v>
       </c>
       <c r="S8" t="n">
-        <v>11.18</v>
+        <v>13.29</v>
       </c>
       <c r="T8" t="n">
-        <v>13.29</v>
+        <v>12.04</v>
       </c>
       <c r="U8" t="n">
-        <v>12.04</v>
+        <v>10</v>
       </c>
       <c r="V8" t="n">
-        <v>10</v>
+        <v>11.94</v>
       </c>
       <c r="W8" t="n">
-        <v>11.94</v>
+        <v>10.84</v>
       </c>
       <c r="X8" t="n">
-        <v>10.84</v>
+        <v>5.970000000000001</v>
       </c>
       <c r="Y8" t="n">
-        <v>5.970000000000001</v>
+        <v>10.67</v>
       </c>
       <c r="Z8" t="n">
-        <v>10.67</v>
+        <v>11.25</v>
       </c>
       <c r="AA8" t="n">
-        <v>11.25</v>
+        <v>11.07</v>
       </c>
       <c r="AB8" t="n">
-        <v>11.07</v>
+        <v>12.16</v>
       </c>
       <c r="AC8" t="n">
-        <v>12.16</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="AD8" t="n">
-        <v>8.640000000000001</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>2.7</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="9">
@@ -1302,7 +1276,7 @@
         <v>10.16</v>
       </c>
       <c r="L9" t="n">
-        <v>9</v>
+        <v>9.69</v>
       </c>
       <c r="M9" t="n">
         <v>7.67</v>
@@ -1323,43 +1297,40 @@
         <v>3.83</v>
       </c>
       <c r="S9" t="n">
-        <v>12.19</v>
+        <v>9.68</v>
       </c>
       <c r="T9" t="n">
-        <v>9.68</v>
+        <v>8.91</v>
       </c>
       <c r="U9" t="n">
-        <v>8.91</v>
+        <v>7.71</v>
       </c>
       <c r="V9" t="n">
-        <v>7.71</v>
+        <v>9.469999999999999</v>
       </c>
       <c r="W9" t="n">
-        <v>9.469999999999999</v>
+        <v>12.14</v>
       </c>
       <c r="X9" t="n">
-        <v>12.14</v>
+        <v>5.809999999999999</v>
       </c>
       <c r="Y9" t="n">
-        <v>5.809999999999999</v>
+        <v>10.98</v>
       </c>
       <c r="Z9" t="n">
-        <v>10.98</v>
+        <v>9.290000000000001</v>
       </c>
       <c r="AA9" t="n">
-        <v>9.290000000000001</v>
+        <v>10.2</v>
       </c>
       <c r="AB9" t="n">
-        <v>10.2</v>
+        <v>12.36</v>
       </c>
       <c r="AC9" t="n">
-        <v>12.36</v>
+        <v>7.02</v>
       </c>
       <c r="AD9" t="n">
-        <v>7.02</v>
-      </c>
-      <c r="AE9" t="n">
-        <v>3.06</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="10">
@@ -1399,7 +1370,7 @@
         <v>10.775</v>
       </c>
       <c r="L10" t="n">
-        <v>10.525</v>
+        <v>10.705</v>
       </c>
       <c r="M10" t="n">
         <v>12.897</v>
@@ -1420,43 +1391,40 @@
         <v>2.141</v>
       </c>
       <c r="S10" t="n">
-        <v>7.892</v>
+        <v>6.512</v>
       </c>
       <c r="T10" t="n">
-        <v>6.512</v>
+        <v>8.402999999999999</v>
       </c>
       <c r="U10" t="n">
-        <v>8.402999999999999</v>
+        <v>12.056</v>
       </c>
       <c r="V10" t="n">
-        <v>12.056</v>
+        <v>8.152999999999999</v>
       </c>
       <c r="W10" t="n">
-        <v>8.152999999999999</v>
+        <v>4.771000000000001</v>
       </c>
       <c r="X10" t="n">
-        <v>4.771000000000001</v>
+        <v>2.631</v>
       </c>
       <c r="Y10" t="n">
+        <v>7.953</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>3.751</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>5.882</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>8.933</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>12.477</v>
+      </c>
+      <c r="AD10" t="n">
         <v>2.631</v>
-      </c>
-      <c r="Z10" t="n">
-        <v>7.953</v>
-      </c>
-      <c r="AA10" t="n">
-        <v>3.751</v>
-      </c>
-      <c r="AB10" t="n">
-        <v>5.882</v>
-      </c>
-      <c r="AC10" t="n">
-        <v>8.933</v>
-      </c>
-      <c r="AD10" t="n">
-        <v>12.477</v>
-      </c>
-      <c r="AE10" t="n">
-        <v>4.032</v>
       </c>
     </row>
     <row r="11">
@@ -1517,43 +1485,40 @@
         <v>3.15</v>
       </c>
       <c r="S11" t="n">
-        <v>10.65</v>
+        <v>12.22</v>
       </c>
       <c r="T11" t="n">
-        <v>12.22</v>
+        <v>11.92</v>
       </c>
       <c r="U11" t="n">
-        <v>11.92</v>
+        <v>10.55</v>
       </c>
       <c r="V11" t="n">
-        <v>10.55</v>
+        <v>11.41</v>
       </c>
       <c r="W11" t="n">
-        <v>11.41</v>
+        <v>9.029999999999999</v>
       </c>
       <c r="X11" t="n">
-        <v>9.029999999999999</v>
+        <v>4.59</v>
       </c>
       <c r="Y11" t="n">
-        <v>4.59</v>
+        <v>9.950000000000001</v>
       </c>
       <c r="Z11" t="n">
-        <v>9.950000000000001</v>
+        <v>9.620000000000003</v>
       </c>
       <c r="AA11" t="n">
-        <v>9.620000000000003</v>
+        <v>9.76</v>
       </c>
       <c r="AB11" t="n">
-        <v>9.76</v>
+        <v>11.36</v>
       </c>
       <c r="AC11" t="n">
-        <v>11.36</v>
+        <v>9.359999999999999</v>
       </c>
       <c r="AD11" t="n">
-        <v>9.359999999999999</v>
-      </c>
-      <c r="AE11" t="n">
-        <v>2.85</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="12">
@@ -1593,7 +1558,7 @@
         <v>9.76</v>
       </c>
       <c r="L12" t="n">
-        <v>8.31</v>
+        <v>8.9</v>
       </c>
       <c r="M12" t="n">
         <v>6.15</v>
@@ -1614,43 +1579,40 @@
         <v>4.640000000000001</v>
       </c>
       <c r="S12" t="n">
-        <v>11.38</v>
+        <v>10.03</v>
       </c>
       <c r="T12" t="n">
-        <v>10.03</v>
+        <v>8.02</v>
       </c>
       <c r="U12" t="n">
-        <v>8.02</v>
+        <v>6.42</v>
       </c>
       <c r="V12" t="n">
-        <v>6.42</v>
+        <v>9.17</v>
       </c>
       <c r="W12" t="n">
-        <v>9.17</v>
+        <v>13.24</v>
       </c>
       <c r="X12" t="n">
-        <v>13.24</v>
+        <v>7.24</v>
       </c>
       <c r="Y12" t="n">
-        <v>7.24</v>
+        <v>10.79</v>
       </c>
       <c r="Z12" t="n">
-        <v>10.79</v>
+        <v>10.47</v>
       </c>
       <c r="AA12" t="n">
-        <v>10.47</v>
+        <v>10.91</v>
       </c>
       <c r="AB12" t="n">
-        <v>10.91</v>
+        <v>12.09</v>
       </c>
       <c r="AC12" t="n">
-        <v>12.09</v>
+        <v>5.71</v>
       </c>
       <c r="AD12" t="n">
-        <v>5.71</v>
-      </c>
-      <c r="AE12" t="n">
-        <v>2.63</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="13">
@@ -1690,7 +1652,7 @@
         <v>10.77</v>
       </c>
       <c r="L13" t="n">
-        <v>10.42</v>
+        <v>10.55</v>
       </c>
       <c r="M13" t="n">
         <v>11.58</v>
@@ -1711,43 +1673,40 @@
         <v>2.11</v>
       </c>
       <c r="S13" t="n">
-        <v>9.68</v>
+        <v>7.85</v>
       </c>
       <c r="T13" t="n">
-        <v>7.85</v>
+        <v>9.609999999999999</v>
       </c>
       <c r="U13" t="n">
-        <v>9.609999999999999</v>
+        <v>11.92</v>
       </c>
       <c r="V13" t="n">
-        <v>11.92</v>
+        <v>9.26</v>
       </c>
       <c r="W13" t="n">
-        <v>9.26</v>
+        <v>5.69</v>
       </c>
       <c r="X13" t="n">
-        <v>5.69</v>
+        <v>3.05</v>
       </c>
       <c r="Y13" t="n">
+        <v>8.359999999999999</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>4.119999999999999</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>6.47</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>10.24</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>10.86</v>
+      </c>
+      <c r="AD13" t="n">
         <v>3.05</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>8.359999999999999</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>4.119999999999999</v>
-      </c>
-      <c r="AB13" t="n">
-        <v>6.47</v>
-      </c>
-      <c r="AC13" t="n">
-        <v>10.24</v>
-      </c>
-      <c r="AD13" t="n">
-        <v>10.86</v>
-      </c>
-      <c r="AE13" t="n">
-        <v>3.87</v>
       </c>
     </row>
     <row r="14">
@@ -1808,43 +1767,40 @@
         <v>2.53</v>
       </c>
       <c r="S14" t="n">
-        <v>10.39</v>
+        <v>11.15</v>
       </c>
       <c r="T14" t="n">
-        <v>11.15</v>
+        <v>11.73</v>
       </c>
       <c r="U14" t="n">
-        <v>11.73</v>
+        <v>11.23</v>
       </c>
       <c r="V14" t="n">
-        <v>11.23</v>
+        <v>10.98</v>
       </c>
       <c r="W14" t="n">
-        <v>10.98</v>
+        <v>7.52</v>
       </c>
       <c r="X14" t="n">
-        <v>7.52</v>
+        <v>3.6</v>
       </c>
       <c r="Y14" t="n">
-        <v>3.6</v>
+        <v>9.359999999999999</v>
       </c>
       <c r="Z14" t="n">
-        <v>9.359999999999999</v>
+        <v>7.879999999999999</v>
       </c>
       <c r="AA14" t="n">
-        <v>7.879999999999999</v>
+        <v>8.58</v>
       </c>
       <c r="AB14" t="n">
-        <v>8.58</v>
+        <v>10.9</v>
       </c>
       <c r="AC14" t="n">
-        <v>10.9</v>
+        <v>10</v>
       </c>
       <c r="AD14" t="n">
-        <v>10</v>
-      </c>
-      <c r="AE14" t="n">
-        <v>3.11</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="15">
@@ -1884,7 +1840,7 @@
         <v>10.01</v>
       </c>
       <c r="L15" t="n">
-        <v>8.359999999999999</v>
+        <v>8.75</v>
       </c>
       <c r="M15" t="n">
         <v>5.65</v>
@@ -1905,43 +1861,40 @@
         <v>4.94</v>
       </c>
       <c r="S15" t="n">
-        <v>10.98</v>
+        <v>10.88</v>
       </c>
       <c r="T15" t="n">
-        <v>10.88</v>
+        <v>8.370000000000001</v>
       </c>
       <c r="U15" t="n">
-        <v>8.370000000000001</v>
+        <v>6.52</v>
       </c>
       <c r="V15" t="n">
-        <v>6.52</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="W15" t="n">
-        <v>9.619999999999999</v>
+        <v>13.29</v>
       </c>
       <c r="X15" t="n">
-        <v>13.29</v>
+        <v>7.84</v>
       </c>
       <c r="Y15" t="n">
-        <v>7.84</v>
+        <v>10.59</v>
       </c>
       <c r="Z15" t="n">
-        <v>10.59</v>
+        <v>11.07</v>
       </c>
       <c r="AA15" t="n">
-        <v>11.07</v>
+        <v>11.26</v>
       </c>
       <c r="AB15" t="n">
-        <v>11.26</v>
+        <v>12.04</v>
       </c>
       <c r="AC15" t="n">
-        <v>12.04</v>
+        <v>5.46</v>
       </c>
       <c r="AD15" t="n">
-        <v>5.46</v>
-      </c>
-      <c r="AE15" t="n">
-        <v>2.43</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="16">
@@ -1981,7 +1934,7 @@
         <v>9.41</v>
       </c>
       <c r="L16" t="n">
-        <v>8.119999999999999</v>
+        <v>8.809999999999999</v>
       </c>
       <c r="M16" t="n">
         <v>6.43</v>
@@ -2002,43 +1955,40 @@
         <v>4.16</v>
       </c>
       <c r="S16" t="n">
-        <v>11.28</v>
+        <v>9.32</v>
       </c>
       <c r="T16" t="n">
-        <v>9.32</v>
+        <v>7.83</v>
       </c>
       <c r="U16" t="n">
-        <v>7.83</v>
+        <v>6.34</v>
       </c>
       <c r="V16" t="n">
+        <v>8.720000000000001</v>
+      </c>
+      <c r="W16" t="n">
+        <v>12.57</v>
+      </c>
+      <c r="X16" t="n">
         <v>6.34</v>
       </c>
-      <c r="W16" t="n">
-        <v>8.720000000000001</v>
-      </c>
-      <c r="X16" t="n">
-        <v>12.57</v>
-      </c>
       <c r="Y16" t="n">
-        <v>6.34</v>
+        <v>10.59</v>
       </c>
       <c r="Z16" t="n">
-        <v>10.59</v>
+        <v>9.809999999999999</v>
       </c>
       <c r="AA16" t="n">
-        <v>9.809999999999999</v>
+        <v>10.3</v>
       </c>
       <c r="AB16" t="n">
-        <v>10.3</v>
+        <v>11.68</v>
       </c>
       <c r="AC16" t="n">
-        <v>11.68</v>
+        <v>5.94</v>
       </c>
       <c r="AD16" t="n">
-        <v>5.94</v>
-      </c>
-      <c r="AE16" t="n">
-        <v>2.67</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="17">
@@ -2078,7 +2028,7 @@
         <v>9.550000000000001</v>
       </c>
       <c r="L17" t="n">
-        <v>8.02</v>
+        <v>8.469999999999999</v>
       </c>
       <c r="M17" t="n">
         <v>5.51</v>
@@ -2099,43 +2049,40 @@
         <v>4.84</v>
       </c>
       <c r="S17" t="n">
-        <v>10.8</v>
+        <v>10.18</v>
       </c>
       <c r="T17" t="n">
-        <v>10.18</v>
+        <v>7.77</v>
       </c>
       <c r="U17" t="n">
-        <v>7.77</v>
+        <v>6.140000000000001</v>
       </c>
       <c r="V17" t="n">
-        <v>6.140000000000001</v>
+        <v>9.1</v>
       </c>
       <c r="W17" t="n">
-        <v>9.1</v>
+        <v>13.11</v>
       </c>
       <c r="X17" t="n">
-        <v>13.11</v>
+        <v>7.7</v>
       </c>
       <c r="Y17" t="n">
-        <v>7.7</v>
+        <v>10.35</v>
       </c>
       <c r="Z17" t="n">
-        <v>10.35</v>
+        <v>10.53</v>
       </c>
       <c r="AA17" t="n">
-        <v>10.53</v>
+        <v>10.88</v>
       </c>
       <c r="AB17" t="n">
-        <v>10.88</v>
+        <v>11.78</v>
       </c>
       <c r="AC17" t="n">
-        <v>11.78</v>
+        <v>5.16</v>
       </c>
       <c r="AD17" t="n">
-        <v>5.16</v>
-      </c>
-      <c r="AE17" t="n">
-        <v>2.43</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="18">
@@ -2196,43 +2143,40 @@
         <v>3.489999999999999</v>
       </c>
       <c r="S18" t="n">
-        <v>10.11</v>
+        <v>12.23</v>
       </c>
       <c r="T18" t="n">
-        <v>12.23</v>
+        <v>11.17</v>
       </c>
       <c r="U18" t="n">
-        <v>11.17</v>
+        <v>9.19</v>
       </c>
       <c r="V18" t="n">
-        <v>9.19</v>
+        <v>10.94</v>
       </c>
       <c r="W18" t="n">
-        <v>10.94</v>
+        <v>9.720000000000001</v>
       </c>
       <c r="X18" t="n">
-        <v>9.720000000000001</v>
+        <v>5.18</v>
       </c>
       <c r="Y18" t="n">
-        <v>5.18</v>
+        <v>9.739999999999998</v>
       </c>
       <c r="Z18" t="n">
-        <v>9.739999999999998</v>
+        <v>10.4</v>
       </c>
       <c r="AA18" t="n">
-        <v>10.4</v>
+        <v>10.08</v>
       </c>
       <c r="AB18" t="n">
-        <v>10.08</v>
+        <v>10.96</v>
       </c>
       <c r="AC18" t="n">
-        <v>10.96</v>
+        <v>8.1</v>
       </c>
       <c r="AD18" t="n">
-        <v>8.1</v>
-      </c>
-      <c r="AE18" t="n">
-        <v>2.43</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="19">
@@ -2272,7 +2216,7 @@
         <v>9.34</v>
       </c>
       <c r="L19" t="n">
-        <v>7.71</v>
+        <v>7.97</v>
       </c>
       <c r="M19" t="n">
         <v>4.86</v>
@@ -2293,43 +2237,40 @@
         <v>4.850000000000001</v>
       </c>
       <c r="S19" t="n">
-        <v>9.970000000000001</v>
+        <v>10.45</v>
       </c>
       <c r="T19" t="n">
-        <v>10.45</v>
+        <v>7.75</v>
       </c>
       <c r="U19" t="n">
-        <v>7.75</v>
+        <v>5.970000000000001</v>
       </c>
       <c r="V19" t="n">
-        <v>5.970000000000001</v>
+        <v>9.08</v>
       </c>
       <c r="W19" t="n">
-        <v>9.08</v>
+        <v>12.52</v>
       </c>
       <c r="X19" t="n">
-        <v>12.52</v>
+        <v>7.81</v>
       </c>
       <c r="Y19" t="n">
-        <v>7.81</v>
+        <v>9.710000000000001</v>
       </c>
       <c r="Z19" t="n">
-        <v>9.710000000000001</v>
+        <v>10.56</v>
       </c>
       <c r="AA19" t="n">
-        <v>10.56</v>
+        <v>10.67</v>
       </c>
       <c r="AB19" t="n">
-        <v>10.67</v>
+        <v>11.19</v>
       </c>
       <c r="AC19" t="n">
-        <v>11.19</v>
+        <v>4.75</v>
       </c>
       <c r="AD19" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="AE19" t="n">
-        <v>2.15</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="20">
@@ -2369,7 +2310,7 @@
         <v>8.98</v>
       </c>
       <c r="L20" t="n">
-        <v>7.65</v>
+        <v>8.050000000000001</v>
       </c>
       <c r="M20" t="n">
         <v>6.12</v>
@@ -2390,43 +2331,40 @@
         <v>2.93</v>
       </c>
       <c r="S20" t="n">
-        <v>9.450000000000001</v>
+        <v>9.510000000000002</v>
       </c>
       <c r="T20" t="n">
-        <v>9.510000000000002</v>
+        <v>8.710000000000001</v>
       </c>
       <c r="U20" t="n">
-        <v>8.710000000000001</v>
+        <v>6.65</v>
       </c>
       <c r="V20" t="n">
-        <v>6.65</v>
+        <v>8.58</v>
       </c>
       <c r="W20" t="n">
-        <v>8.58</v>
+        <v>9.52</v>
       </c>
       <c r="X20" t="n">
-        <v>9.52</v>
+        <v>4.13</v>
       </c>
       <c r="Y20" t="n">
-        <v>4.13</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="Z20" t="n">
-        <v>9.050000000000001</v>
+        <v>9.18</v>
       </c>
       <c r="AA20" t="n">
-        <v>9.18</v>
+        <v>8.85</v>
       </c>
       <c r="AB20" t="n">
-        <v>8.85</v>
+        <v>9.65</v>
       </c>
       <c r="AC20" t="n">
-        <v>9.65</v>
+        <v>6.449999999999999</v>
       </c>
       <c r="AD20" t="n">
-        <v>6.449999999999999</v>
-      </c>
-      <c r="AE20" t="n">
-        <v>2.13</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="21">
@@ -2487,42 +2425,39 @@
         <v>4.81</v>
       </c>
       <c r="S21" t="n">
+        <v>10.87</v>
+      </c>
+      <c r="T21" t="n">
+        <v>7.83</v>
+      </c>
+      <c r="U21" t="n">
+        <v>5.81</v>
+      </c>
+      <c r="V21" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="W21" t="n">
+        <v>11.64</v>
+      </c>
+      <c r="X21" t="n">
+        <v>7.85</v>
+      </c>
+      <c r="Y21" t="n">
         <v>8.85</v>
       </c>
-      <c r="T21" t="n">
-        <v>10.87</v>
-      </c>
-      <c r="U21" t="n">
-        <v>7.83</v>
-      </c>
-      <c r="V21" t="n">
-        <v>5.81</v>
-      </c>
-      <c r="W21" t="n">
-        <v>9.1</v>
-      </c>
-      <c r="X21" t="n">
-        <v>11.64</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>7.85</v>
-      </c>
       <c r="Z21" t="n">
-        <v>8.85</v>
+        <v>10.62</v>
       </c>
       <c r="AA21" t="n">
-        <v>10.62</v>
+        <v>10.37</v>
       </c>
       <c r="AB21" t="n">
         <v>10.37</v>
       </c>
       <c r="AC21" t="n">
-        <v>10.37</v>
+        <v>4.29</v>
       </c>
       <c r="AD21" t="n">
-        <v>4.29</v>
-      </c>
-      <c r="AE21" t="n">
         <v>1.77</v>
       </c>
     </row>
@@ -2584,42 +2519,39 @@
         <v>4.03</v>
       </c>
       <c r="S22" t="n">
+        <v>9.31</v>
+      </c>
+      <c r="T22" t="n">
+        <v>6.79</v>
+      </c>
+      <c r="U22" t="n">
+        <v>5.03</v>
+      </c>
+      <c r="V22" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="W22" t="n">
+        <v>9.82</v>
+      </c>
+      <c r="X22" t="n">
+        <v>6.55</v>
+      </c>
+      <c r="Y22" t="n">
         <v>7.55</v>
       </c>
-      <c r="T22" t="n">
-        <v>9.31</v>
-      </c>
-      <c r="U22" t="n">
-        <v>6.79</v>
-      </c>
-      <c r="V22" t="n">
-        <v>5.03</v>
-      </c>
-      <c r="W22" t="n">
-        <v>7.8</v>
-      </c>
-      <c r="X22" t="n">
-        <v>9.82</v>
-      </c>
-      <c r="Y22" t="n">
-        <v>6.55</v>
-      </c>
       <c r="Z22" t="n">
-        <v>7.55</v>
+        <v>9.06</v>
       </c>
       <c r="AA22" t="n">
-        <v>9.06</v>
+        <v>8.81</v>
       </c>
       <c r="AB22" t="n">
         <v>8.81</v>
       </c>
       <c r="AC22" t="n">
-        <v>8.81</v>
+        <v>3.77</v>
       </c>
       <c r="AD22" t="n">
-        <v>3.77</v>
-      </c>
-      <c r="AE22" t="n">
         <v>1.51</v>
       </c>
     </row>
@@ -2660,7 +2592,7 @@
         <v>6.050000000000001</v>
       </c>
       <c r="L23" t="n">
-        <v>5.4</v>
+        <v>5.5</v>
       </c>
       <c r="M23" t="n">
         <v>4.5</v>
@@ -2681,43 +2613,40 @@
         <v>1.87</v>
       </c>
       <c r="S23" t="n">
-        <v>6.47</v>
+        <v>6.08</v>
       </c>
       <c r="T23" t="n">
-        <v>6.08</v>
+        <v>5.9</v>
       </c>
       <c r="U23" t="n">
-        <v>5.9</v>
+        <v>5.37</v>
       </c>
       <c r="V23" t="n">
-        <v>5.37</v>
+        <v>5.95</v>
       </c>
       <c r="W23" t="n">
-        <v>5.95</v>
+        <v>5.51</v>
       </c>
       <c r="X23" t="n">
-        <v>5.51</v>
+        <v>2.989999999999999</v>
       </c>
       <c r="Y23" t="n">
-        <v>2.989999999999999</v>
+        <v>5.529999999999999</v>
       </c>
       <c r="Z23" t="n">
-        <v>5.529999999999999</v>
+        <v>4.62</v>
       </c>
       <c r="AA23" t="n">
-        <v>4.62</v>
+        <v>5.26</v>
       </c>
       <c r="AB23" t="n">
-        <v>5.26</v>
+        <v>6.72</v>
       </c>
       <c r="AC23" t="n">
-        <v>6.72</v>
+        <v>4.28</v>
       </c>
       <c r="AD23" t="n">
-        <v>4.28</v>
-      </c>
-      <c r="AE23" t="n">
-        <v>1.69</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="24">
@@ -2778,43 +2707,40 @@
         <v>10.68</v>
       </c>
       <c r="S24" t="n">
+        <v>5.08</v>
+      </c>
+      <c r="T24" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="U24" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="V24" t="n">
+        <v>5.96</v>
+      </c>
+      <c r="W24" t="n">
+        <v>5.68</v>
+      </c>
+      <c r="X24" t="n">
+        <v>11.88</v>
+      </c>
+      <c r="Y24" t="n">
         <v>4.48</v>
       </c>
-      <c r="T24" t="n">
+      <c r="Z24" t="n">
         <v>5.08</v>
-      </c>
-      <c r="U24" t="n">
-        <v>3.88</v>
-      </c>
-      <c r="V24" t="n">
-        <v>3.28</v>
-      </c>
-      <c r="W24" t="n">
-        <v>5.96</v>
-      </c>
-      <c r="X24" t="n">
-        <v>5.68</v>
-      </c>
-      <c r="Y24" t="n">
-        <v>11.88</v>
-      </c>
-      <c r="Z24" t="n">
-        <v>4.48</v>
       </c>
       <c r="AA24" t="n">
         <v>5.08</v>
       </c>
       <c r="AB24" t="n">
-        <v>5.08</v>
+        <v>6.56</v>
       </c>
       <c r="AC24" t="n">
-        <v>6.56</v>
+        <v>2.68</v>
       </c>
       <c r="AD24" t="n">
-        <v>2.68</v>
-      </c>
-      <c r="AE24" t="n">
-        <v>3.56</v>
+        <v>2.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>